<commit_message>
Planning En Assetlist Update 2.0
title
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarloAkuma\Documents\Gamelab\Deltion.Gamelab1\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarloAkuma\Desktop\JOHN CENA TUUTUUDUU TUUU\Gamelab1\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="330">
   <si>
     <t>Planning</t>
   </si>
@@ -666,13 +666,361 @@
   </si>
   <si>
     <t>7S_TTA_001</t>
+  </si>
+  <si>
+    <t>Week 45</t>
+  </si>
+  <si>
+    <t>Week 46</t>
+  </si>
+  <si>
+    <t>week 47</t>
+  </si>
+  <si>
+    <t>Week 48</t>
+  </si>
+  <si>
+    <t>Week 49</t>
+  </si>
+  <si>
+    <t>Week 50</t>
+  </si>
+  <si>
+    <t>Week 51</t>
+  </si>
+  <si>
+    <t>Week 53</t>
+  </si>
+  <si>
+    <t>Week 52</t>
+  </si>
+  <si>
+    <t>Week 54</t>
+  </si>
+  <si>
+    <t>WeeK 55</t>
+  </si>
+  <si>
+    <t>Planning Volgende Periode</t>
+  </si>
+  <si>
+    <t>2D_ENEQANT_001</t>
+  </si>
+  <si>
+    <t>3D_ENEQANT_001</t>
+  </si>
+  <si>
+    <t>4U_ENEQANT_001</t>
+  </si>
+  <si>
+    <t>2D_WSWORD_001</t>
+  </si>
+  <si>
+    <t>3D_WSWORD_001</t>
+  </si>
+  <si>
+    <t>4U_WSWORD_001</t>
+  </si>
+  <si>
+    <t>6A_EGW_001</t>
+  </si>
+  <si>
+    <t>6A_EGA_001</t>
+  </si>
+  <si>
+    <t>6A_DFW_001</t>
+  </si>
+  <si>
+    <t>6A_DFA_001</t>
+  </si>
+  <si>
+    <t>6A_SRHW_001</t>
+  </si>
+  <si>
+    <t>6A_SRHS_001</t>
+  </si>
+  <si>
+    <t>6A_SHRI_001</t>
+  </si>
+  <si>
+    <t>6A_SHRD_001</t>
+  </si>
+  <si>
+    <t>6A_SHRJ_001</t>
+  </si>
+  <si>
+    <t>6A_SHRT_001</t>
+  </si>
+  <si>
+    <t>6A_SHRSW_001</t>
+  </si>
+  <si>
+    <t>6A_SHRSW_002</t>
+  </si>
+  <si>
+    <t>6A_SHRSW_003</t>
+  </si>
+  <si>
+    <t>6A_SHRSW_004</t>
+  </si>
+  <si>
+    <t>6A_SHRSW_005</t>
+  </si>
+  <si>
+    <t>6A_SHRSW_006</t>
+  </si>
+  <si>
+    <t>6A_SRCS_001</t>
+  </si>
+  <si>
+    <t>6A_SRKI_001</t>
+  </si>
+  <si>
+    <t>6A_SRAW_001</t>
+  </si>
+  <si>
+    <t>6A_SRAS_001</t>
+  </si>
+  <si>
+    <t>6A_SRAS_002</t>
+  </si>
+  <si>
+    <t>6A_SRAS_003</t>
+  </si>
+  <si>
+    <t>6A_SRAS_004</t>
+  </si>
+  <si>
+    <t>6A_SRADJ_001</t>
+  </si>
+  <si>
+    <t>6A_SRAI_001</t>
+  </si>
+  <si>
+    <t>6A_SRCE_001</t>
+  </si>
+  <si>
+    <t>2D_ENVJL_001</t>
+  </si>
+  <si>
+    <t>3D_ENVJL_001</t>
+  </si>
+  <si>
+    <t>4U_ENVJL_001</t>
+  </si>
+  <si>
+    <t>2D_ENVRL_001</t>
+  </si>
+  <si>
+    <t>3D_ENVRL_001</t>
+  </si>
+  <si>
+    <t>4U_ENVRL_001</t>
+  </si>
+  <si>
+    <t>2D_ENVRO_001</t>
+  </si>
+  <si>
+    <t>3D_ENVRO_001</t>
+  </si>
+  <si>
+    <t>4u_ENVRO_001</t>
+  </si>
+  <si>
+    <t>2D_ENVJP_001</t>
+  </si>
+  <si>
+    <t>3D_ENVJP_001</t>
+  </si>
+  <si>
+    <t>4U_ENVJP_001</t>
+  </si>
+  <si>
+    <t>2D_ENVLINE_001</t>
+  </si>
+  <si>
+    <t>3D_ENVLINE_001</t>
+  </si>
+  <si>
+    <t>4U_ENVLINE_001</t>
+  </si>
+  <si>
+    <t>2D_ENVCLO_001</t>
+  </si>
+  <si>
+    <t>3D_ENVCLO_001</t>
+  </si>
+  <si>
+    <t>4U_ENVCLO_001</t>
+  </si>
+  <si>
+    <t>4U_ENVDESK_001</t>
+  </si>
+  <si>
+    <t>2D_ENVDESK_001</t>
+  </si>
+  <si>
+    <t>3D_ENVDESK_001</t>
+  </si>
+  <si>
+    <t>2D_ENVBED_001</t>
+  </si>
+  <si>
+    <t>3D_ENVBED_001</t>
+  </si>
+  <si>
+    <t>4U_ENVBED_001</t>
+  </si>
+  <si>
+    <t>2D_ENVPIL_001</t>
+  </si>
+  <si>
+    <t>3D_ENVPIL_001</t>
+  </si>
+  <si>
+    <t>4U_ENVPIL_001</t>
+  </si>
+  <si>
+    <t>2D_ENVNS_001</t>
+  </si>
+  <si>
+    <t>3D_ENVNS_001</t>
+  </si>
+  <si>
+    <t>4U_ENVNS_001</t>
+  </si>
+  <si>
+    <t>2D_ENVTRAINR_001</t>
+  </si>
+  <si>
+    <t>3D_ENVTRAINR_001</t>
+  </si>
+  <si>
+    <t>4U_ENVTRAINR_001</t>
+  </si>
+  <si>
+    <t>3D_ENVTOYTR_001</t>
+  </si>
+  <si>
+    <t>4U_ENVTOYTR_001</t>
+  </si>
+  <si>
+    <t>2D_EnVTOYTR_001</t>
+  </si>
+  <si>
+    <t>2D_ENVRAMP_001</t>
+  </si>
+  <si>
+    <t>3D_ENVRAMP_001</t>
+  </si>
+  <si>
+    <t>4U_ENVRAMP_001</t>
+  </si>
+  <si>
+    <t>2D_ENVTUBE_001</t>
+  </si>
+  <si>
+    <t>3D_ENVTUBE_001</t>
+  </si>
+  <si>
+    <t>4U_ENVTUBE_001</t>
+  </si>
+  <si>
+    <t>2D_ENVCHAIR_001</t>
+  </si>
+  <si>
+    <t>3D_ENVCHAIR_001</t>
+  </si>
+  <si>
+    <t>4U_ENVCHAIR_001</t>
+  </si>
+  <si>
+    <t>2D_ENVTP_001</t>
+  </si>
+  <si>
+    <t>4U_ENVTP_001</t>
+  </si>
+  <si>
+    <t>3D_ENVTP_001</t>
+  </si>
+  <si>
+    <t>2D_ENVSPARE_001</t>
+  </si>
+  <si>
+    <t>3D_ENVSPARE_001</t>
+  </si>
+  <si>
+    <t>4U_ENVSPARE_001</t>
+  </si>
+  <si>
+    <t>2D_ENVJP_002</t>
+  </si>
+  <si>
+    <t>3D_ENVJP_002</t>
+  </si>
+  <si>
+    <t>4U_ENVJP_002</t>
+  </si>
+  <si>
+    <t>2D_ENVTABLE_001</t>
+  </si>
+  <si>
+    <t>3D_ENVTABLE_001</t>
+  </si>
+  <si>
+    <t>4U_ENVTABLE_001</t>
+  </si>
+  <si>
+    <t>3D_ENVSPWALL_001</t>
+  </si>
+  <si>
+    <t>4U_ENVSPWALL_001</t>
+  </si>
+  <si>
+    <t>2D_ENVSPWALL_001</t>
+  </si>
+  <si>
+    <t>2D_ENVTNT_001</t>
+  </si>
+  <si>
+    <t>3D_ENVTNT_001</t>
+  </si>
+  <si>
+    <t>4U_ENVTNT_001</t>
+  </si>
+  <si>
+    <t>6A_SRKG_001</t>
+  </si>
+  <si>
+    <t>6A_SRKL_001</t>
+  </si>
+  <si>
+    <t>BUFFER WEEK</t>
+  </si>
+  <si>
+    <t>6A_EAW_001</t>
+  </si>
+  <si>
+    <t>6A_EAA_001</t>
+  </si>
+  <si>
+    <t>6A_ELW_001</t>
+  </si>
+  <si>
+    <t>6A_ELA_001</t>
+  </si>
+  <si>
+    <t>6A_SRSP_001</t>
+  </si>
+  <si>
+    <t>6A_SRSG_001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +1045,27 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -890,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -934,6 +1303,11 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -963,8 +1337,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF7C80"/>
       <color rgb="FF00FFFF"/>
-      <color rgb="FFFF7C80"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1241,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC143"/>
+  <dimension ref="A2:AC200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H114" sqref="G114:H114"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H157" sqref="H156:H157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4514,10 +4888,10 @@
     <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="2"/>
-      <c r="C97" s="4" t="s">
+      <c r="C97" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D97" s="2"/>
+      <c r="D97" s="1"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -4582,10 +4956,10 @@
     <row r="99" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
       <c r="B99" s="2"/>
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D99" s="2"/>
+      <c r="D99" s="1"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -4614,10 +4988,10 @@
     <row r="100" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="2"/>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D100" s="2"/>
+      <c r="D100" s="1"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -5014,10 +5388,10 @@
     <row r="112" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="4"/>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="D112" s="2"/>
+      <c r="D112" s="30"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="42" t="s">
@@ -5058,10 +5432,10 @@
     <row r="113" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
       <c r="B113" s="2"/>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D113" s="2"/>
+      <c r="D113" s="30"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="1" t="s">
@@ -5098,10 +5472,10 @@
     <row r="114" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="2"/>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="D114" s="2"/>
+      <c r="D114" s="30"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="1" t="s">
@@ -5138,10 +5512,10 @@
     <row r="115" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A115" s="10"/>
       <c r="B115" s="2"/>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="D115" s="2"/>
+      <c r="D115" s="32"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
@@ -5176,10 +5550,10 @@
     <row r="116" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="10"/>
       <c r="B116" s="2"/>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="D116" s="2"/>
+      <c r="D116" s="32"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
@@ -5211,13 +5585,13 @@
       </c>
       <c r="AB116" s="11"/>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="10"/>
       <c r="B117" s="2"/>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="D117" s="2"/>
+      <c r="D117" s="32"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -5232,133 +5606,152 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
       <c r="R117" s="2"/>
-      <c r="S117" s="2" t="s">
-        <v>157</v>
-      </c>
+      <c r="S117" s="2"/>
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>
       <c r="V117" s="2"/>
-      <c r="W117" s="1" t="s">
-        <v>160</v>
-      </c>
+      <c r="W117" s="1"/>
       <c r="X117" s="1"/>
       <c r="Y117" s="2"/>
       <c r="Z117" s="2"/>
-      <c r="AA117" s="1" t="s">
+      <c r="AA117" s="1"/>
+      <c r="AB117" s="11"/>
+    </row>
+    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A118" s="10"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D118" s="4"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+      <c r="L118" s="2"/>
+      <c r="M118" s="2"/>
+      <c r="N118" s="2"/>
+      <c r="O118" s="2"/>
+      <c r="P118" s="2"/>
+      <c r="Q118" s="2"/>
+      <c r="R118" s="2"/>
+      <c r="S118" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="T118" s="2"/>
+      <c r="U118" s="2"/>
+      <c r="V118" s="2"/>
+      <c r="W118" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="X118" s="1"/>
+      <c r="Y118" s="2"/>
+      <c r="Z118" s="2"/>
+      <c r="AA118" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AB117" s="11"/>
-    </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A118" s="23"/>
-      <c r="B118" s="24" t="s">
+      <c r="AB118" s="11"/>
+    </row>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A119" s="23"/>
+      <c r="B119" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C118" s="24"/>
-      <c r="D118" s="24"/>
-      <c r="E118" s="24"/>
-      <c r="F118" s="24" t="s">
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G118" s="24"/>
-      <c r="H118" s="24"/>
-      <c r="I118" s="24"/>
-      <c r="J118" s="24" t="s">
+      <c r="G119" s="24"/>
+      <c r="H119" s="24"/>
+      <c r="I119" s="24"/>
+      <c r="J119" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="K118" s="24"/>
-      <c r="L118" s="24"/>
-      <c r="M118" s="24"/>
-      <c r="N118" s="24" t="s">
+      <c r="K119" s="24"/>
+      <c r="L119" s="24"/>
+      <c r="M119" s="24"/>
+      <c r="N119" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="O118" s="24"/>
-      <c r="P118" s="24"/>
-      <c r="Q118" s="24"/>
-      <c r="R118" s="24"/>
-      <c r="S118" s="24" t="s">
+      <c r="O119" s="24"/>
+      <c r="P119" s="24"/>
+      <c r="Q119" s="24"/>
+      <c r="R119" s="24"/>
+      <c r="S119" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="T118" s="24"/>
-      <c r="U118" s="24"/>
-      <c r="V118" s="24"/>
-      <c r="W118" s="24" t="s">
+      <c r="T119" s="24"/>
+      <c r="U119" s="24"/>
+      <c r="V119" s="24"/>
+      <c r="W119" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="X118" s="24"/>
-      <c r="Y118" s="24"/>
-      <c r="Z118" s="24" t="s">
+      <c r="X119" s="24"/>
+      <c r="Y119" s="24"/>
+      <c r="Z119" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA118" s="24"/>
-      <c r="AB118" s="25"/>
-    </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A119" s="4"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
-      <c r="G119" s="4"/>
-      <c r="H119" s="4"/>
-      <c r="I119" s="4"/>
-      <c r="J119" s="4"/>
-      <c r="K119" s="4"/>
-      <c r="L119" s="4"/>
-      <c r="M119" s="4"/>
-      <c r="N119" s="4"/>
-      <c r="O119" s="4"/>
-      <c r="P119" s="4"/>
-      <c r="Q119" s="4"/>
-      <c r="R119" s="4"/>
-      <c r="S119" s="4"/>
-      <c r="T119" s="4"/>
-      <c r="U119" s="4"/>
-      <c r="V119" s="4"/>
-      <c r="W119" s="4"/>
-      <c r="X119" s="4"/>
-      <c r="Y119" s="4"/>
-      <c r="Z119" s="4"/>
-      <c r="AA119" s="4"/>
-      <c r="AB119" s="4"/>
-      <c r="AC119" s="2"/>
-    </row>
-    <row r="120" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="4"/>
-      <c r="J120" s="4"/>
-      <c r="K120" s="4"/>
-      <c r="L120" s="4"/>
-      <c r="M120" s="4"/>
-      <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
-      <c r="R120" s="4"/>
-      <c r="S120" s="4"/>
-      <c r="T120" s="4"/>
-      <c r="U120" s="4"/>
-      <c r="V120" s="4"/>
-      <c r="W120" s="4"/>
-      <c r="X120" s="4"/>
-      <c r="Y120" s="4"/>
-      <c r="Z120" s="4"/>
-      <c r="AA120" s="4"/>
-      <c r="AB120" s="4"/>
+      <c r="AA119" s="24"/>
+      <c r="AB119" s="25"/>
+    </row>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L120" s="6"/>
+      <c r="M120" s="6"/>
+      <c r="N120" s="6"/>
+      <c r="O120" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P120" s="6"/>
+      <c r="Q120" s="6"/>
+      <c r="R120" s="6"/>
+      <c r="S120" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T120" s="6"/>
+      <c r="U120" s="6"/>
+      <c r="V120" s="6"/>
+      <c r="W120" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X120" s="6"/>
+      <c r="Y120" s="6"/>
+      <c r="Z120" s="6"/>
+      <c r="AA120" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB120" s="15"/>
       <c r="AC120" s="2"/>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A121" s="4"/>
+    <row r="121" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="10"/>
       <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
+      <c r="C121" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
@@ -5374,11 +5767,15 @@
       <c r="P121" s="4"/>
       <c r="Q121" s="4"/>
       <c r="R121" s="4"/>
-      <c r="S121" s="4"/>
+      <c r="S121" s="4" t="s">
+        <v>227</v>
+      </c>
       <c r="T121" s="4"/>
       <c r="U121" s="4"/>
       <c r="V121" s="4"/>
-      <c r="W121" s="4"/>
+      <c r="W121" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="X121" s="4"/>
       <c r="Y121" s="4"/>
       <c r="Z121" s="4"/>
@@ -5387,9 +5784,11 @@
       <c r="AC121" s="2"/>
     </row>
     <row r="122" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A122" s="4"/>
+      <c r="A122" s="10"/>
       <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
+      <c r="C122" s="4" t="s">
+        <v>229</v>
+      </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
@@ -5405,11 +5804,15 @@
       <c r="P122" s="4"/>
       <c r="Q122" s="4"/>
       <c r="R122" s="4"/>
-      <c r="S122" s="4"/>
+      <c r="S122" s="4" t="s">
+        <v>228</v>
+      </c>
       <c r="T122" s="4"/>
       <c r="U122" s="4"/>
       <c r="V122" s="4"/>
-      <c r="W122" s="4"/>
+      <c r="W122" s="4" t="s">
+        <v>235</v>
+      </c>
       <c r="X122" s="4"/>
       <c r="Y122" s="4"/>
       <c r="Z122" s="4"/>
@@ -5418,9 +5821,11 @@
       <c r="AC122" s="2"/>
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
+      <c r="A123" s="10"/>
       <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
+      <c r="C123" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
@@ -5436,7 +5841,9 @@
       <c r="P123" s="4"/>
       <c r="Q123" s="4"/>
       <c r="R123" s="4"/>
-      <c r="S123" s="4"/>
+      <c r="S123" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="T123" s="4"/>
       <c r="U123" s="4"/>
       <c r="V123" s="4"/>
@@ -5449,9 +5856,11 @@
       <c r="AC123" s="2"/>
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
+      <c r="A124" s="10"/>
       <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
+      <c r="C124" s="4" t="s">
+        <v>231</v>
+      </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
@@ -5467,7 +5876,9 @@
       <c r="P124" s="4"/>
       <c r="Q124" s="4"/>
       <c r="R124" s="4"/>
-      <c r="S124" s="4"/>
+      <c r="S124" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="T124" s="4"/>
       <c r="U124" s="4"/>
       <c r="V124" s="4"/>
@@ -5480,9 +5891,11 @@
       <c r="AC124" s="2"/>
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
+      <c r="A125" s="10"/>
       <c r="B125" s="4"/>
-      <c r="C125" s="4"/>
+      <c r="C125" s="4" t="s">
+        <v>236</v>
+      </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
@@ -5511,9 +5924,11 @@
       <c r="AC125" s="2"/>
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
+      <c r="A126" s="10"/>
       <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
+      <c r="C126" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
@@ -5542,7 +5957,7 @@
       <c r="AC126" s="2"/>
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
+      <c r="A127" s="10"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
@@ -5573,7 +5988,7 @@
       <c r="AC127" s="2"/>
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A128" s="4"/>
+      <c r="A128" s="10"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -5604,7 +6019,7 @@
       <c r="AC128" s="2"/>
     </row>
     <row r="129" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A129" s="4"/>
+      <c r="A129" s="10"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
@@ -5635,7 +6050,7 @@
       <c r="AC129" s="2"/>
     </row>
     <row r="130" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A130" s="4"/>
+      <c r="A130" s="6"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
@@ -5666,7 +6081,7 @@
       <c r="AC130" s="2"/>
     </row>
     <row r="131" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A131" s="4"/>
+      <c r="A131" s="43"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -5697,40 +6112,58 @@
       <c r="AC131" s="2"/>
     </row>
     <row r="132" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A132" s="4"/>
-      <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="4"/>
-      <c r="E132" s="4"/>
-      <c r="F132" s="4"/>
-      <c r="G132" s="4"/>
-      <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="4"/>
-      <c r="K132" s="4"/>
-      <c r="L132" s="4"/>
-      <c r="M132" s="4"/>
-      <c r="N132" s="4"/>
-      <c r="O132" s="4"/>
-      <c r="P132" s="4"/>
-      <c r="Q132" s="4"/>
-      <c r="R132" s="4"/>
-      <c r="S132" s="4"/>
-      <c r="T132" s="4"/>
-      <c r="U132" s="4"/>
-      <c r="V132" s="4"/>
-      <c r="W132" s="4"/>
-      <c r="X132" s="4"/>
-      <c r="Y132" s="4"/>
-      <c r="Z132" s="4"/>
-      <c r="AA132" s="4"/>
-      <c r="AB132" s="4"/>
+      <c r="A132" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B132" s="6"/>
+      <c r="C132" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H132" s="6"/>
+      <c r="I132" s="6"/>
+      <c r="J132" s="6"/>
+      <c r="K132" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L132" s="6"/>
+      <c r="M132" s="6"/>
+      <c r="N132" s="6"/>
+      <c r="O132" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P132" s="6"/>
+      <c r="Q132" s="6"/>
+      <c r="R132" s="6"/>
+      <c r="S132" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T132" s="6"/>
+      <c r="U132" s="6"/>
+      <c r="V132" s="6"/>
+      <c r="W132" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X132" s="6"/>
+      <c r="Y132" s="6"/>
+      <c r="Z132" s="6"/>
+      <c r="AA132" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB132" s="15"/>
       <c r="AC132" s="2"/>
     </row>
-    <row r="133" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="4"/>
+    <row r="133" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A133" s="10"/>
       <c r="B133" s="4"/>
-      <c r="C133" s="4"/>
+      <c r="C133" s="4" t="s">
+        <v>238</v>
+      </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
@@ -5746,11 +6179,15 @@
       <c r="P133" s="4"/>
       <c r="Q133" s="4"/>
       <c r="R133" s="4"/>
-      <c r="S133" s="4"/>
+      <c r="S133" s="4" t="s">
+        <v>257</v>
+      </c>
       <c r="T133" s="4"/>
       <c r="U133" s="4"/>
       <c r="V133" s="4"/>
-      <c r="W133" s="4"/>
+      <c r="W133" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="X133" s="4"/>
       <c r="Y133" s="4"/>
       <c r="Z133" s="4"/>
@@ -5759,9 +6196,11 @@
       <c r="AC133" s="2"/>
     </row>
     <row r="134" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A134" s="4"/>
+      <c r="A134" s="10"/>
       <c r="B134" s="4"/>
-      <c r="C134" s="4"/>
+      <c r="C134" s="4" t="s">
+        <v>239</v>
+      </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
@@ -5781,7 +6220,9 @@
       <c r="T134" s="4"/>
       <c r="U134" s="4"/>
       <c r="V134" s="4"/>
-      <c r="W134" s="4"/>
+      <c r="W134" s="4" t="s">
+        <v>249</v>
+      </c>
       <c r="X134" s="4"/>
       <c r="Y134" s="4"/>
       <c r="Z134" s="4"/>
@@ -5790,7 +6231,7 @@
       <c r="AC134" s="2"/>
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A135" s="4"/>
+      <c r="A135" s="10"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
@@ -5821,7 +6262,7 @@
       <c r="AC135" s="2"/>
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A136" s="4"/>
+      <c r="A136" s="10"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
@@ -5852,7 +6293,7 @@
       <c r="AC136" s="2"/>
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A137" s="4"/>
+      <c r="A137" s="10"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
@@ -5883,7 +6324,7 @@
       <c r="AC137" s="2"/>
     </row>
     <row r="138" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A138" s="4"/>
+      <c r="A138" s="10"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
@@ -5913,41 +6354,59 @@
       <c r="AB138" s="4"/>
       <c r="AC138" s="2"/>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
-      <c r="E139" s="4"/>
-      <c r="F139" s="4"/>
-      <c r="G139" s="4"/>
-      <c r="H139" s="4"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="4"/>
-      <c r="O139" s="4"/>
-      <c r="P139" s="4"/>
-      <c r="Q139" s="4"/>
-      <c r="R139" s="4"/>
-      <c r="S139" s="4"/>
-      <c r="T139" s="4"/>
-      <c r="U139" s="4"/>
-      <c r="V139" s="4"/>
-      <c r="W139" s="4"/>
-      <c r="X139" s="4"/>
-      <c r="Y139" s="4"/>
-      <c r="Z139" s="4"/>
-      <c r="AA139" s="4"/>
-      <c r="AB139" s="4"/>
+    <row r="139" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6"/>
+      <c r="J139" s="6"/>
+      <c r="K139" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L139" s="6"/>
+      <c r="M139" s="6"/>
+      <c r="N139" s="6"/>
+      <c r="O139" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P139" s="6"/>
+      <c r="Q139" s="6"/>
+      <c r="R139" s="6"/>
+      <c r="S139" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T139" s="6"/>
+      <c r="U139" s="6"/>
+      <c r="V139" s="6"/>
+      <c r="W139" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X139" s="6"/>
+      <c r="Y139" s="6"/>
+      <c r="Z139" s="6"/>
+      <c r="AA139" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB139" s="15"/>
       <c r="AC139" s="2"/>
     </row>
     <row r="140" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A140" s="4"/>
+      <c r="A140" s="10"/>
       <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
+      <c r="C140" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
@@ -5963,11 +6422,15 @@
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
       <c r="R140" s="4"/>
-      <c r="S140" s="4"/>
+      <c r="S140" s="4" t="s">
+        <v>249</v>
+      </c>
       <c r="T140" s="4"/>
       <c r="U140" s="4"/>
       <c r="V140" s="4"/>
-      <c r="W140" s="4"/>
+      <c r="W140" s="4" t="s">
+        <v>250</v>
+      </c>
       <c r="X140" s="4"/>
       <c r="Y140" s="4"/>
       <c r="Z140" s="4"/>
@@ -5976,9 +6439,11 @@
       <c r="AC140" s="2"/>
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A141" s="4"/>
+      <c r="A141" s="10"/>
       <c r="B141" s="4"/>
-      <c r="C141" s="4"/>
+      <c r="C141" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
@@ -5994,11 +6459,15 @@
       <c r="P141" s="4"/>
       <c r="Q141" s="4"/>
       <c r="R141" s="4"/>
-      <c r="S141" s="4"/>
+      <c r="S141" s="4" t="s">
+        <v>258</v>
+      </c>
       <c r="T141" s="4"/>
       <c r="U141" s="4"/>
       <c r="V141" s="4"/>
-      <c r="W141" s="4"/>
+      <c r="W141" s="4" t="s">
+        <v>251</v>
+      </c>
       <c r="X141" s="4"/>
       <c r="Y141" s="4"/>
       <c r="Z141" s="4"/>
@@ -6007,7 +6476,7 @@
       <c r="AC141" s="2"/>
     </row>
     <row r="142" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A142" s="4"/>
+      <c r="A142" s="10"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
@@ -6025,11 +6494,15 @@
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
       <c r="R142" s="4"/>
-      <c r="S142" s="4"/>
+      <c r="S142" s="4" t="s">
+        <v>259</v>
+      </c>
       <c r="T142" s="4"/>
       <c r="U142" s="4"/>
       <c r="V142" s="4"/>
-      <c r="W142" s="4"/>
+      <c r="W142" s="4" t="s">
+        <v>252</v>
+      </c>
       <c r="X142" s="4"/>
       <c r="Y142" s="4"/>
       <c r="Z142" s="4"/>
@@ -6038,35 +6511,1024 @@
       <c r="AC142" s="2"/>
     </row>
     <row r="143" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
-      <c r="I143" s="2"/>
-      <c r="J143" s="2"/>
-      <c r="K143" s="2"/>
-      <c r="L143" s="2"/>
-      <c r="M143" s="2"/>
-      <c r="N143" s="2"/>
-      <c r="O143" s="2"/>
-      <c r="P143" s="2"/>
-      <c r="Q143" s="2"/>
-      <c r="R143" s="2"/>
-      <c r="S143" s="2"/>
-      <c r="T143" s="2"/>
-      <c r="U143" s="2"/>
-      <c r="V143" s="2"/>
-      <c r="W143" s="2"/>
-      <c r="X143" s="2"/>
-      <c r="Y143" s="2"/>
-      <c r="Z143" s="2"/>
-      <c r="AA143" s="2"/>
-      <c r="AB143" s="2"/>
+      <c r="A143" s="43"/>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="4"/>
+      <c r="I143" s="4"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="4"/>
+      <c r="L143" s="4"/>
+      <c r="M143" s="4"/>
+      <c r="N143" s="4"/>
+      <c r="O143" s="4"/>
+      <c r="P143" s="4"/>
+      <c r="Q143" s="4"/>
+      <c r="R143" s="4"/>
+      <c r="S143" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="T143" s="4"/>
+      <c r="U143" s="4"/>
+      <c r="V143" s="4"/>
+      <c r="W143" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="X143" s="4"/>
+      <c r="Y143" s="4"/>
+      <c r="Z143" s="4"/>
+      <c r="AA143" s="4"/>
+      <c r="AB143" s="4"/>
       <c r="AC143" s="2"/>
+    </row>
+    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A144" s="43"/>
+      <c r="B144" s="4"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="4"/>
+      <c r="I144" s="4"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="4"/>
+      <c r="L144" s="4"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="4"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="4"/>
+      <c r="Q144" s="4"/>
+      <c r="R144" s="4"/>
+      <c r="S144" s="4"/>
+      <c r="T144" s="4"/>
+      <c r="U144" s="4"/>
+      <c r="V144" s="4"/>
+      <c r="W144" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="X144" s="4"/>
+      <c r="Y144" s="4"/>
+      <c r="Z144" s="4"/>
+      <c r="AA144" s="4"/>
+      <c r="AB144" s="4"/>
+      <c r="AC144" s="2"/>
+    </row>
+    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A145" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H145" s="6"/>
+      <c r="I145" s="6"/>
+      <c r="J145" s="6"/>
+      <c r="K145" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L145" s="6"/>
+      <c r="M145" s="6"/>
+      <c r="N145" s="6"/>
+      <c r="O145" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P145" s="6"/>
+      <c r="Q145" s="6"/>
+      <c r="R145" s="6"/>
+      <c r="S145" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T145" s="6"/>
+      <c r="U145" s="6"/>
+      <c r="V145" s="6"/>
+      <c r="W145" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X145" s="6"/>
+      <c r="Y145" s="6"/>
+      <c r="Z145" s="6"/>
+      <c r="AA145" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB145" s="15"/>
+      <c r="AC145" s="2"/>
+    </row>
+    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A146" s="44"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+      <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="4"/>
+      <c r="L146" s="4"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="4"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="4"/>
+      <c r="Q146" s="4"/>
+      <c r="R146" s="4"/>
+      <c r="S146" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="T146" s="4"/>
+      <c r="U146" s="4"/>
+      <c r="V146" s="4"/>
+      <c r="W146" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="X146" s="4"/>
+      <c r="Y146" s="4"/>
+      <c r="Z146" s="4"/>
+      <c r="AA146" s="4"/>
+      <c r="AB146" s="4"/>
+      <c r="AC146" s="2"/>
+    </row>
+    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A147" s="43"/>
+      <c r="B147" s="4"/>
+      <c r="C147" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
+      <c r="H147" s="4"/>
+      <c r="I147" s="4"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="4"/>
+      <c r="L147" s="4"/>
+      <c r="M147" s="4"/>
+      <c r="N147" s="4"/>
+      <c r="O147" s="4"/>
+      <c r="P147" s="4"/>
+      <c r="Q147" s="4"/>
+      <c r="R147" s="4"/>
+      <c r="S147" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="T147" s="4"/>
+      <c r="U147" s="4"/>
+      <c r="V147" s="4"/>
+      <c r="W147" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="X147" s="4"/>
+      <c r="Y147" s="4"/>
+      <c r="Z147" s="4"/>
+      <c r="AA147" s="4"/>
+      <c r="AB147" s="4"/>
+      <c r="AC147" s="2"/>
+    </row>
+    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A148" s="10"/>
+      <c r="B148" s="4"/>
+      <c r="C148" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
+      <c r="H148" s="4"/>
+      <c r="I148" s="4"/>
+      <c r="J148" s="4"/>
+      <c r="K148" s="4"/>
+      <c r="L148" s="4"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="4"/>
+      <c r="O148" s="4"/>
+      <c r="P148" s="4"/>
+      <c r="Q148" s="4"/>
+      <c r="R148" s="4"/>
+      <c r="S148" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="T148" s="4"/>
+      <c r="U148" s="4"/>
+      <c r="V148" s="4"/>
+      <c r="W148" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="X148" s="4"/>
+      <c r="Y148" s="4"/>
+      <c r="Z148" s="4"/>
+      <c r="AA148" s="4"/>
+      <c r="AB148" s="4"/>
+      <c r="AC148" s="2"/>
+    </row>
+    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A149" s="10"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D149" s="2"/>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+      <c r="H149" s="2"/>
+      <c r="I149" s="2"/>
+      <c r="J149" s="2"/>
+      <c r="K149" s="2"/>
+      <c r="L149" s="2"/>
+      <c r="M149" s="2"/>
+      <c r="N149" s="2"/>
+      <c r="O149" s="2"/>
+      <c r="P149" s="2"/>
+      <c r="Q149" s="2"/>
+      <c r="R149" s="2"/>
+      <c r="S149" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="T149" s="2"/>
+      <c r="U149" s="2"/>
+      <c r="V149" s="2"/>
+      <c r="W149" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="X149" s="2"/>
+      <c r="Y149" s="2"/>
+      <c r="Z149" s="2"/>
+      <c r="AA149" s="2"/>
+      <c r="AB149" s="2"/>
+      <c r="AC149" s="2"/>
+    </row>
+    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A150" s="10"/>
+      <c r="C150" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="W150" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A151" s="10"/>
+      <c r="C151" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="W151" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A152" s="10"/>
+    </row>
+    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A153" s="43" t="s">
+        <v>218</v>
+      </c>
+      <c r="B153" s="6"/>
+      <c r="C153" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D153" s="6"/>
+      <c r="E153" s="6"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H153" s="6"/>
+      <c r="I153" s="6"/>
+      <c r="J153" s="6"/>
+      <c r="K153" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L153" s="6"/>
+      <c r="M153" s="6"/>
+      <c r="N153" s="6"/>
+      <c r="O153" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P153" s="6"/>
+      <c r="Q153" s="6"/>
+      <c r="R153" s="6"/>
+      <c r="S153" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T153" s="6"/>
+      <c r="U153" s="6"/>
+      <c r="V153" s="6"/>
+      <c r="W153" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X153" s="6"/>
+      <c r="Y153" s="6"/>
+      <c r="Z153" s="6"/>
+      <c r="AA153" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB153" s="15"/>
+    </row>
+    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A154" s="10"/>
+      <c r="C154" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D154" s="4"/>
+      <c r="S154" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="T154" s="4"/>
+      <c r="W154" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A155" s="43"/>
+      <c r="C155" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D155" s="4"/>
+      <c r="S155" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="T155" s="4"/>
+      <c r="W155" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A156" s="10"/>
+      <c r="C156" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D156" s="4"/>
+      <c r="S156" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="T156" s="4"/>
+    </row>
+    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A157" s="10"/>
+      <c r="C157" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D157" s="4"/>
+    </row>
+    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A158" s="43"/>
+    </row>
+    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A159" s="10"/>
+    </row>
+    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A160" s="10"/>
+    </row>
+    <row r="161" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A161" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D161" s="6"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H161" s="6"/>
+      <c r="I161" s="6"/>
+      <c r="J161" s="6"/>
+      <c r="K161" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L161" s="6"/>
+      <c r="M161" s="6"/>
+      <c r="N161" s="6"/>
+      <c r="O161" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P161" s="6"/>
+      <c r="Q161" s="6"/>
+      <c r="R161" s="6"/>
+      <c r="S161" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T161" s="6"/>
+      <c r="U161" s="6"/>
+      <c r="V161" s="6"/>
+      <c r="W161" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X161" s="6"/>
+      <c r="Y161" s="6"/>
+      <c r="Z161" s="6"/>
+      <c r="AA161" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB161" s="15"/>
+    </row>
+    <row r="162" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A162" s="10"/>
+      <c r="C162" t="s">
+        <v>273</v>
+      </c>
+      <c r="S162" t="s">
+        <v>264</v>
+      </c>
+      <c r="W162" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="163" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A163" s="10"/>
+      <c r="C163" t="s">
+        <v>274</v>
+      </c>
+      <c r="S163" t="s">
+        <v>265</v>
+      </c>
+      <c r="W163" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="164" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A164" s="10"/>
+      <c r="C164" t="s">
+        <v>275</v>
+      </c>
+      <c r="S164" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="165" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A165" s="10"/>
+      <c r="C165" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="166" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A166" s="10"/>
+      <c r="C166" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="167" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A167" s="10"/>
+      <c r="C167" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="168" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A168" s="10"/>
+    </row>
+    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A169" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D169" s="6"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="6"/>
+      <c r="G169" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H169" s="6"/>
+      <c r="I169" s="6"/>
+      <c r="J169" s="6"/>
+      <c r="K169" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L169" s="6"/>
+      <c r="M169" s="6"/>
+      <c r="N169" s="6"/>
+      <c r="O169" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P169" s="6"/>
+      <c r="Q169" s="6"/>
+      <c r="R169" s="6"/>
+      <c r="S169" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T169" s="6"/>
+      <c r="U169" s="6"/>
+      <c r="V169" s="6"/>
+      <c r="W169" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X169" s="6"/>
+      <c r="Y169" s="6"/>
+      <c r="Z169" s="6"/>
+      <c r="AA169" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB169" s="15"/>
+    </row>
+    <row r="170" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A170" s="10"/>
+      <c r="C170" t="s">
+        <v>279</v>
+      </c>
+      <c r="S170" t="s">
+        <v>309</v>
+      </c>
+      <c r="W170" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A171" s="10"/>
+      <c r="C171" t="s">
+        <v>280</v>
+      </c>
+      <c r="S171" t="s">
+        <v>310</v>
+      </c>
+      <c r="W171" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="172" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A172" s="10"/>
+      <c r="C172" t="s">
+        <v>281</v>
+      </c>
+      <c r="S172" t="s">
+        <v>311</v>
+      </c>
+      <c r="W172" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="173" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A173" s="10"/>
+      <c r="C173" t="s">
+        <v>282</v>
+      </c>
+      <c r="S173" t="s">
+        <v>312</v>
+      </c>
+      <c r="W173" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="174" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A174" s="10"/>
+      <c r="C174" t="s">
+        <v>283</v>
+      </c>
+      <c r="S174" t="s">
+        <v>313</v>
+      </c>
+      <c r="W174" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="175" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A175" s="10"/>
+      <c r="C175" t="s">
+        <v>284</v>
+      </c>
+      <c r="S175" t="s">
+        <v>314</v>
+      </c>
+      <c r="W175" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="176" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A176" s="10"/>
+    </row>
+    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A177" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="B177" s="6"/>
+      <c r="C177" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H177" s="6"/>
+      <c r="I177" s="6"/>
+      <c r="J177" s="6"/>
+      <c r="K177" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L177" s="6"/>
+      <c r="M177" s="6"/>
+      <c r="N177" s="6"/>
+      <c r="O177" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P177" s="6"/>
+      <c r="Q177" s="6"/>
+      <c r="R177" s="6"/>
+      <c r="S177" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T177" s="6"/>
+      <c r="U177" s="6"/>
+      <c r="V177" s="6"/>
+      <c r="W177" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X177" s="6"/>
+      <c r="Y177" s="6"/>
+      <c r="Z177" s="6"/>
+      <c r="AA177" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB177" s="15"/>
+    </row>
+    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A178" s="10"/>
+      <c r="C178" t="s">
+        <v>285</v>
+      </c>
+      <c r="S178" t="s">
+        <v>318</v>
+      </c>
+      <c r="W178" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A179" s="10"/>
+      <c r="C179" t="s">
+        <v>286</v>
+      </c>
+      <c r="S179" t="s">
+        <v>319</v>
+      </c>
+      <c r="W179" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A180" s="10"/>
+      <c r="C180" t="s">
+        <v>287</v>
+      </c>
+      <c r="S180" t="s">
+        <v>320</v>
+      </c>
+      <c r="W180" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A181" s="10"/>
+      <c r="C181" t="s">
+        <v>288</v>
+      </c>
+      <c r="W181" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A182" s="10"/>
+      <c r="C182" t="s">
+        <v>289</v>
+      </c>
+      <c r="W182" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="183" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A183" s="10"/>
+      <c r="C183" t="s">
+        <v>290</v>
+      </c>
+      <c r="W183" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A184" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D184" s="6"/>
+      <c r="E184" s="6"/>
+      <c r="F184" s="6"/>
+      <c r="G184" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H184" s="6"/>
+      <c r="I184" s="6"/>
+      <c r="J184" s="6"/>
+      <c r="K184" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L184" s="6"/>
+      <c r="M184" s="6"/>
+      <c r="N184" s="6"/>
+      <c r="O184" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P184" s="6"/>
+      <c r="Q184" s="6"/>
+      <c r="R184" s="6"/>
+      <c r="S184" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T184" s="6"/>
+      <c r="U184" s="6"/>
+      <c r="V184" s="6"/>
+      <c r="W184" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X184" s="6"/>
+      <c r="Y184" s="6"/>
+      <c r="Z184" s="6"/>
+      <c r="AA184" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB184" s="15"/>
+    </row>
+    <row r="185" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A185" s="10"/>
+      <c r="C185" t="s">
+        <v>293</v>
+      </c>
+      <c r="S185" t="s">
+        <v>324</v>
+      </c>
+      <c r="W185" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="186" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A186" s="10"/>
+      <c r="C186" t="s">
+        <v>291</v>
+      </c>
+      <c r="S186" t="s">
+        <v>325</v>
+      </c>
+      <c r="W186" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="187" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A187" s="10"/>
+      <c r="C187" t="s">
+        <v>292</v>
+      </c>
+      <c r="S187" t="s">
+        <v>326</v>
+      </c>
+      <c r="W187" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="188" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A188" s="10"/>
+      <c r="S188" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="189" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A189" s="10"/>
+    </row>
+    <row r="190" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A190" s="10"/>
+    </row>
+    <row r="191" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A191" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B191" s="6"/>
+      <c r="C191" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D191" s="6"/>
+      <c r="E191" s="6"/>
+      <c r="F191" s="6"/>
+      <c r="G191" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H191" s="6"/>
+      <c r="I191" s="6"/>
+      <c r="J191" s="6"/>
+      <c r="K191" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L191" s="6"/>
+      <c r="M191" s="6"/>
+      <c r="N191" s="6"/>
+      <c r="O191" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P191" s="6"/>
+      <c r="Q191" s="6"/>
+      <c r="R191" s="6"/>
+      <c r="S191" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T191" s="6"/>
+      <c r="U191" s="6"/>
+      <c r="V191" s="6"/>
+      <c r="W191" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X191" s="6"/>
+      <c r="Y191" s="6"/>
+      <c r="Z191" s="6"/>
+      <c r="AA191" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB191" s="15"/>
+    </row>
+    <row r="192" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A192" s="10"/>
+      <c r="C192" t="s">
+        <v>317</v>
+      </c>
+      <c r="W192" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="193" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A193" s="10"/>
+      <c r="C193" t="s">
+        <v>315</v>
+      </c>
+      <c r="W193" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="194" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A194" s="10"/>
+      <c r="C194" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="195" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A195" s="10"/>
+    </row>
+    <row r="196" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A196" s="10"/>
+    </row>
+    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A197" s="10"/>
+    </row>
+    <row r="198" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A198" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B198" s="6"/>
+      <c r="C198" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D198" s="6"/>
+      <c r="E198" s="6"/>
+      <c r="F198" s="6"/>
+      <c r="G198" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H198" s="6"/>
+      <c r="I198" s="6"/>
+      <c r="J198" s="6"/>
+      <c r="K198" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L198" s="6"/>
+      <c r="M198" s="6"/>
+      <c r="N198" s="6"/>
+      <c r="O198" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P198" s="6"/>
+      <c r="Q198" s="6"/>
+      <c r="R198" s="6"/>
+      <c r="S198" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T198" s="6"/>
+      <c r="U198" s="6"/>
+      <c r="V198" s="6"/>
+      <c r="W198" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X198" s="6"/>
+      <c r="Y198" s="6"/>
+      <c r="Z198" s="6"/>
+      <c r="AA198" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB198" s="15"/>
+    </row>
+    <row r="199" spans="1:28" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A199" s="10"/>
+      <c r="B199" s="45"/>
+      <c r="C199" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="D199" s="47"/>
+      <c r="E199" s="47"/>
+      <c r="F199" s="47"/>
+      <c r="G199" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="H199" s="47"/>
+      <c r="I199" s="47"/>
+      <c r="J199" s="47"/>
+      <c r="K199" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="L199" s="47"/>
+      <c r="M199" s="47"/>
+      <c r="N199" s="47"/>
+      <c r="O199" s="47"/>
+      <c r="P199" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q199" s="47"/>
+      <c r="R199" s="47"/>
+      <c r="S199" s="47"/>
+      <c r="T199" s="47"/>
+      <c r="U199" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="V199" s="47"/>
+      <c r="W199" s="47"/>
+      <c r="X199" s="47"/>
+      <c r="Y199" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="Z199" s="47"/>
+      <c r="AA199" s="47"/>
+      <c r="AB199" s="47"/>
+    </row>
+    <row r="200" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A200" s="23"/>
+      <c r="B200" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C200" s="24"/>
+      <c r="D200" s="24"/>
+      <c r="E200" s="24"/>
+      <c r="F200" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G200" s="24"/>
+      <c r="H200" s="24"/>
+      <c r="I200" s="24"/>
+      <c r="J200" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K200" s="24"/>
+      <c r="L200" s="24"/>
+      <c r="M200" s="24"/>
+      <c r="N200" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="O200" s="24"/>
+      <c r="P200" s="24"/>
+      <c r="Q200" s="24"/>
+      <c r="R200" s="24"/>
+      <c r="S200" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="T200" s="24"/>
+      <c r="U200" s="24"/>
+      <c r="V200" s="24"/>
+      <c r="W200" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="X200" s="24"/>
+      <c r="Y200" s="24"/>
+      <c r="Z200" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA200" s="24"/>
+      <c r="AB200" s="25"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="V54:X56 W59:W62 W64:W69">

</xml_diff>

<commit_message>
Planning en de Asset , Toolbox en je moeder
Je moeder riijmt op asset
-rief 2015
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarloAkuma\Desktop\JOHN CENA TUUTUUDUU TUUU\Gamelab1\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarloAkuma\Desktop\Gamelab 1\Gamelab1\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="362">
   <si>
     <t>Planning</t>
   </si>
@@ -695,12 +695,6 @@
     <t>Week 52</t>
   </si>
   <si>
-    <t>Week 54</t>
-  </si>
-  <si>
-    <t>WeeK 55</t>
-  </si>
-  <si>
     <t>Planning Volgende Periode</t>
   </si>
   <si>
@@ -968,9 +962,6 @@
     <t>6A_SRKL_001</t>
   </si>
   <si>
-    <t>BUFFER WEEK</t>
-  </si>
-  <si>
     <t>6A_EAW_001</t>
   </si>
   <si>
@@ -1022,9 +1013,6 @@
     <t>Particles Onderzoeken</t>
   </si>
   <si>
-    <t>Lvl 2 Fien</t>
-  </si>
-  <si>
     <t>7S_SAL_001</t>
   </si>
   <si>
@@ -1053,13 +1041,82 @@
   </si>
   <si>
     <t>Level 3 testing</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>WeeK 2</t>
+  </si>
+  <si>
+    <t>VAKANTIE VAKANTIE VAKANTIE VAKANTIE VAKANTIE VAKANTIE VAKANTIE</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Lvl 2 Fixen</t>
+  </si>
+  <si>
+    <t>Lvl Design met marc</t>
+  </si>
+  <si>
+    <t>Particle's gemaakt</t>
+  </si>
+  <si>
+    <t>STORY BOARDING</t>
+  </si>
+  <si>
+    <t>2D_KSWORD_001</t>
+  </si>
+  <si>
+    <t>3D_KSWORD_001</t>
+  </si>
+  <si>
+    <t>4U_KSWORD_001</t>
+  </si>
+  <si>
+    <t>2D_ASWORD_001</t>
+  </si>
+  <si>
+    <t>3D_ASWORD_001</t>
+  </si>
+  <si>
+    <t>4U_ASWORD_001</t>
+  </si>
+  <si>
+    <t>2D_CGUNS_001</t>
+  </si>
+  <si>
+    <t>3D_CGUNS_001</t>
+  </si>
+  <si>
+    <t>4U_CGUNS_001</t>
+  </si>
+  <si>
+    <t>6A_SRHSP_001</t>
+  </si>
+  <si>
+    <t>Scripts Samenleggen</t>
+  </si>
+  <si>
+    <t>Presentatie Maken</t>
+  </si>
+  <si>
+    <t>Presentatie Doornemen</t>
+  </si>
+  <si>
+    <t>Level Design FT. Marc</t>
+  </si>
+  <si>
+    <t>Level Design FT. Danial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1104,6 +1161,13 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1298,7 +1362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1341,10 +1405,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1652,10 +1719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC207"/>
+  <dimension ref="A2:AC209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A176" activeCellId="1" sqref="A184 A176"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W171" sqref="W171:X171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4064,10 +4131,10 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
-      <c r="S72" s="40" t="s">
+      <c r="S72" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T72" s="40"/>
+      <c r="T72" s="1"/>
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
       <c r="W72" s="1" t="s">
@@ -4084,10 +4151,10 @@
     <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="2"/>
-      <c r="C73" s="40" t="s">
+      <c r="C73" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D73" s="40"/>
+      <c r="D73" s="1"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="1" t="s">
@@ -4106,10 +4173,10 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
-      <c r="S73" s="40" t="s">
+      <c r="S73" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T73" s="40"/>
+      <c r="T73" s="1"/>
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
       <c r="W73" s="1" t="s">
@@ -4286,10 +4353,10 @@
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
       <c r="R78" s="2"/>
-      <c r="S78" s="40" t="s">
+      <c r="S78" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="T78" s="40"/>
+      <c r="T78" s="1"/>
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
       <c r="W78" s="2"/>
@@ -4318,10 +4385,10 @@
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
       <c r="R79" s="2"/>
-      <c r="S79" s="40" t="s">
+      <c r="S79" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="T79" s="40"/>
+      <c r="T79" s="1"/>
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
@@ -4626,10 +4693,10 @@
       <c r="D89" s="31"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
-      <c r="G89" s="40" t="s">
+      <c r="G89" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H89" s="40"/>
+      <c r="H89" s="1"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2" t="s">
@@ -5440,10 +5507,10 @@
       <c r="H112" s="40"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
-      <c r="K112" s="2" t="s">
+      <c r="K112" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L112" s="2"/>
+      <c r="L112" s="1"/>
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
       <c r="O112" s="2" t="s">
@@ -5452,10 +5519,10 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
       <c r="R112" s="2"/>
-      <c r="S112" s="2" t="s">
+      <c r="S112" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="T112" s="2"/>
+      <c r="T112" s="1"/>
       <c r="U112" s="2"/>
       <c r="V112" s="2"/>
       <c r="W112" s="1" t="s">
@@ -5492,10 +5559,10 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
       <c r="R113" s="2"/>
-      <c r="S113" s="2" t="s">
+      <c r="S113" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="T113" s="2"/>
+      <c r="T113" s="1"/>
       <c r="U113" s="2"/>
       <c r="V113" s="2"/>
       <c r="W113" s="1" t="s">
@@ -5532,10 +5599,10 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
       <c r="R114" s="2"/>
-      <c r="S114" s="2" t="s">
+      <c r="S114" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="T114" s="2"/>
+      <c r="T114" s="1"/>
       <c r="U114" s="2"/>
       <c r="V114" s="2"/>
       <c r="W114" s="1" t="s">
@@ -5570,10 +5637,10 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
       <c r="R115" s="2"/>
-      <c r="S115" s="2" t="s">
+      <c r="S115" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="T115" s="2"/>
+      <c r="T115" s="1"/>
       <c r="U115" s="2"/>
       <c r="V115" s="2"/>
       <c r="W115" s="1" t="s">
@@ -5608,10 +5675,10 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
       <c r="R116" s="2"/>
-      <c r="S116" s="2" t="s">
+      <c r="S116" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="T116" s="2"/>
+      <c r="T116" s="1"/>
       <c r="U116" s="2"/>
       <c r="V116" s="2"/>
       <c r="W116" s="1" t="s">
@@ -5661,7 +5728,7 @@
       <c r="A118" s="10"/>
       <c r="B118" s="2"/>
       <c r="C118" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="2"/>
@@ -5789,60 +5856,59 @@
     <row r="121" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
       <c r="B121" s="4"/>
-      <c r="C121" s="4" t="s">
-        <v>226</v>
-      </c>
+      <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
-      <c r="G121" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="H121" s="4"/>
+      <c r="G121" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H121" s="1"/>
       <c r="I121" s="4"/>
       <c r="J121" s="4"/>
-      <c r="K121" s="4" t="s">
+      <c r="K121" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L121" s="4"/>
+      <c r="L121" s="1"/>
       <c r="M121" s="4"/>
-      <c r="N121" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="O121" s="4"/>
+      <c r="N121" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="O121" s="1"/>
       <c r="P121" s="4"/>
       <c r="Q121" s="4"/>
       <c r="R121" s="4"/>
-      <c r="S121" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="T121" s="4"/>
+      <c r="S121" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="T121" s="1"/>
       <c r="U121" s="4"/>
       <c r="V121" s="4"/>
-      <c r="W121" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="X121" s="4"/>
+      <c r="W121" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="X121" s="1"/>
       <c r="Y121" s="4"/>
       <c r="Z121" s="4"/>
-      <c r="AA121" s="4" t="s">
-        <v>332</v>
-      </c>
+      <c r="AA121" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AB121" s="18"/>
       <c r="AC121" s="2"/>
     </row>
     <row r="122" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="4"/>
       <c r="C122" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
-      <c r="G122" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="H122" s="4"/>
+      <c r="G122" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H122" s="1"/>
       <c r="I122" s="4"/>
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
@@ -5853,16 +5919,16 @@
       <c r="P122" s="4"/>
       <c r="Q122" s="4"/>
       <c r="R122" s="4"/>
-      <c r="S122" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="T122" s="4"/>
+      <c r="S122" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="T122" s="1"/>
       <c r="U122" s="4"/>
       <c r="V122" s="4"/>
-      <c r="W122" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="X122" s="4"/>
+      <c r="W122" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="X122" s="1"/>
       <c r="Y122" s="4"/>
       <c r="Z122" s="4"/>
       <c r="AC122" s="2"/>
@@ -5871,7 +5937,7 @@
       <c r="A123" s="10"/>
       <c r="B123" s="4"/>
       <c r="C123" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="4"/>
@@ -5888,16 +5954,16 @@
       <c r="P123" s="4"/>
       <c r="Q123" s="4"/>
       <c r="R123" s="4"/>
-      <c r="S123" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="T123" s="4"/>
+      <c r="S123" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="T123" s="1"/>
       <c r="U123" s="4"/>
       <c r="V123" s="4"/>
-      <c r="W123" s="4" t="s">
+      <c r="W123" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="X123" s="4"/>
+      <c r="X123" s="1"/>
       <c r="Y123" s="4"/>
       <c r="Z123" s="4"/>
       <c r="AC123" s="2"/>
@@ -5906,7 +5972,7 @@
       <c r="A124" s="10"/>
       <c r="B124" s="4"/>
       <c r="C124" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="4"/>
@@ -5923,14 +5989,14 @@
       <c r="P124" s="4"/>
       <c r="Q124" s="4"/>
       <c r="R124" s="4"/>
-      <c r="S124" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="T124" s="4"/>
+      <c r="S124" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="T124" s="1"/>
       <c r="U124" s="4"/>
       <c r="V124" s="4"/>
       <c r="W124" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="Y124" s="4"/>
       <c r="Z124" s="4"/>
@@ -5941,10 +6007,10 @@
     <row r="125" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A125" s="10"/>
       <c r="B125" s="4"/>
-      <c r="C125" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D125" s="4"/>
+      <c r="C125" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D125" s="1"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
@@ -5963,10 +6029,10 @@
       <c r="T125" s="4"/>
       <c r="U125" s="4"/>
       <c r="V125" s="4"/>
-      <c r="W125" s="44" t="s">
-        <v>310</v>
-      </c>
-      <c r="X125" s="44"/>
+      <c r="W125" s="43" t="s">
+        <v>308</v>
+      </c>
+      <c r="X125" s="43"/>
       <c r="Y125" s="4"/>
       <c r="Z125" s="4"/>
       <c r="AA125" s="4"/>
@@ -5976,10 +6042,10 @@
     <row r="126" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
       <c r="B126" s="4"/>
-      <c r="C126" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D126" s="4"/>
+      <c r="C126" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D126" s="1"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
@@ -5998,10 +6064,10 @@
       <c r="T126" s="4"/>
       <c r="U126" s="4"/>
       <c r="V126" s="4"/>
-      <c r="W126" s="44" t="s">
-        <v>311</v>
-      </c>
-      <c r="X126" s="44"/>
+      <c r="W126" s="43" t="s">
+        <v>309</v>
+      </c>
+      <c r="X126" s="43"/>
       <c r="Y126" s="4"/>
       <c r="Z126" s="4"/>
       <c r="AA126" s="4"/>
@@ -6207,62 +6273,65 @@
     <row r="133" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A133" s="10"/>
       <c r="B133" s="4"/>
-      <c r="C133" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D133" s="4"/>
+      <c r="C133" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D133" s="1"/>
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
-      <c r="G133" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="H133" s="4"/>
+      <c r="G133" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H133" s="1"/>
       <c r="I133" s="4"/>
       <c r="J133" s="4"/>
-      <c r="K133" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="L133" s="4"/>
+      <c r="K133" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="L133" s="18"/>
       <c r="M133" s="4"/>
       <c r="N133" s="4"/>
-      <c r="O133" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="P133" s="4"/>
+      <c r="O133" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="P133" s="1"/>
       <c r="Q133" s="4"/>
       <c r="R133" s="4"/>
-      <c r="S133" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="T133" s="4"/>
+      <c r="S133" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="T133" s="1"/>
       <c r="U133" s="4"/>
       <c r="V133" s="4"/>
-      <c r="W133" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="X133" s="4"/>
+      <c r="W133" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="X133" s="1"/>
       <c r="Y133" s="4"/>
       <c r="Z133" s="4"/>
-      <c r="AA133" t="s">
-        <v>315</v>
-      </c>
+      <c r="AA133" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="AB133" s="18"/>
       <c r="AC133" s="2"/>
     </row>
     <row r="134" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A134" s="10"/>
       <c r="B134" s="4"/>
-      <c r="C134" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="D134" s="4"/>
+      <c r="C134" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D134" s="1"/>
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
       <c r="J134" s="4"/>
-      <c r="K134" s="4"/>
-      <c r="L134" s="4"/>
+      <c r="K134" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="L134" s="1"/>
       <c r="M134" s="4"/>
       <c r="N134" s="4"/>
       <c r="O134" s="4"/>
@@ -6273,15 +6342,16 @@
       <c r="T134" s="4"/>
       <c r="U134" s="4"/>
       <c r="V134" s="4"/>
-      <c r="W134" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="X134" s="4"/>
+      <c r="W134" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="X134" s="1"/>
       <c r="Y134" s="4"/>
       <c r="Z134" s="4"/>
-      <c r="AA134" t="s">
-        <v>316</v>
-      </c>
+      <c r="AA134" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="AB134" s="18"/>
       <c r="AC134" s="2"/>
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.25">
@@ -6295,8 +6365,10 @@
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
       <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
-      <c r="L135" s="4"/>
+      <c r="K135" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="L135" s="1"/>
       <c r="M135" s="4"/>
       <c r="N135" s="4"/>
       <c r="O135" s="4"/>
@@ -6311,10 +6383,10 @@
       <c r="X135" s="4"/>
       <c r="Y135" s="4"/>
       <c r="Z135" s="4"/>
-      <c r="AA135" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="AB135" s="4"/>
+      <c r="AA135" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB135" s="1"/>
       <c r="AC135" s="2"/>
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.25">
@@ -6344,17 +6416,17 @@
       <c r="X136" s="4"/>
       <c r="Y136" s="4"/>
       <c r="Z136" s="4"/>
-      <c r="AA136" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="AB136" s="21"/>
+      <c r="AA136" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="AB136" s="1"/>
       <c r="AC136" s="2"/>
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A137" s="10"/>
       <c r="B137" s="21"/>
       <c r="C137" s="21" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D137" s="21"/>
       <c r="E137" s="21"/>
@@ -6372,19 +6444,19 @@
       <c r="Q137" s="21"/>
       <c r="R137" s="21"/>
       <c r="S137" s="21" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="T137" s="21"/>
       <c r="U137" s="21"/>
       <c r="V137" s="21"/>
       <c r="W137" s="21" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="X137" s="21"/>
       <c r="Y137" s="21"/>
       <c r="Z137" s="21"/>
       <c r="AA137" s="21" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AB137" s="21"/>
       <c r="AC137" s="2"/>
@@ -6563,55 +6635,55 @@
     <row r="143" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A143" s="10"/>
       <c r="B143" s="4"/>
-      <c r="C143" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="D143" s="4"/>
+      <c r="C143" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D143" s="1"/>
       <c r="E143" s="4"/>
       <c r="F143" s="4"/>
-      <c r="G143" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="H143" s="4"/>
+      <c r="G143" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H143" s="1"/>
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
       <c r="K143" s="4" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="L143" s="4"/>
       <c r="M143" s="4"/>
       <c r="N143" s="4"/>
       <c r="O143" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="P143" s="4"/>
       <c r="Q143" s="4"/>
       <c r="R143" s="4"/>
-      <c r="S143" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="T143" s="4"/>
+      <c r="S143" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="T143" s="1"/>
       <c r="U143" s="4"/>
       <c r="V143" s="4"/>
-      <c r="W143" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="X143" s="4"/>
+      <c r="W143" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="X143" s="1"/>
       <c r="Y143" s="4"/>
       <c r="Z143" s="4"/>
-      <c r="AA143" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="AB143" s="4"/>
+      <c r="AA143" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="AB143" s="5"/>
       <c r="AC143" s="2"/>
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A144" s="10"/>
       <c r="B144" s="4"/>
-      <c r="C144" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D144" s="4"/>
+      <c r="C144" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D144" s="1"/>
       <c r="E144" s="4"/>
       <c r="F144" s="4"/>
       <c r="G144" s="4"/>
@@ -6626,29 +6698,31 @@
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
       <c r="R144" s="4"/>
-      <c r="S144" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="T144" s="4"/>
+      <c r="S144" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="T144" s="1"/>
       <c r="U144" s="4"/>
       <c r="V144" s="4"/>
-      <c r="W144" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="X144" s="4"/>
+      <c r="W144" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="X144" s="1"/>
       <c r="Y144" s="4"/>
       <c r="Z144" s="4"/>
-      <c r="AA144" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="AB144" s="4"/>
+      <c r="AA144" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AB144" s="5"/>
       <c r="AC144" s="2"/>
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A145" s="6"/>
       <c r="B145" s="4"/>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
+      <c r="C145" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="D145" s="18"/>
       <c r="E145" s="4"/>
       <c r="F145" s="4"/>
       <c r="G145" s="4"/>
@@ -6663,29 +6737,31 @@
       <c r="P145" s="4"/>
       <c r="Q145" s="4"/>
       <c r="R145" s="4"/>
-      <c r="S145" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="T145" s="4"/>
+      <c r="S145" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="T145" s="1"/>
       <c r="U145" s="4"/>
       <c r="V145" s="4"/>
-      <c r="W145" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="X145" s="4"/>
+      <c r="W145" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="X145" s="1"/>
       <c r="Y145" s="4"/>
       <c r="Z145" s="4"/>
-      <c r="AA145" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AB145" s="4"/>
+      <c r="AA145" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB145" s="5"/>
       <c r="AC145" s="2"/>
     </row>
     <row r="146" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A146" s="6"/>
       <c r="B146" s="4"/>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
+      <c r="C146" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D146" s="18"/>
       <c r="E146" s="4"/>
       <c r="F146" s="4"/>
       <c r="G146" s="4"/>
@@ -6700,29 +6776,29 @@
       <c r="P146" s="4"/>
       <c r="Q146" s="4"/>
       <c r="R146" s="4"/>
-      <c r="S146" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="T146" s="4"/>
+      <c r="S146" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T146" s="1"/>
       <c r="U146" s="4"/>
       <c r="V146" s="4"/>
-      <c r="W146" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="X146" s="4"/>
+      <c r="W146" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="X146" s="1"/>
       <c r="Y146" s="4"/>
       <c r="Z146" s="4"/>
-      <c r="AA146" s="4" t="s">
-        <v>268</v>
-      </c>
+      <c r="AA146" s="4"/>
       <c r="AB146" s="4"/>
       <c r="AC146" s="2"/>
     </row>
     <row r="147" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A147" s="6"/>
       <c r="B147" s="4"/>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+      <c r="C147" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D147" s="18"/>
       <c r="E147" s="4"/>
       <c r="F147" s="4"/>
       <c r="G147" s="4"/>
@@ -6741,23 +6817,23 @@
       <c r="T147" s="4"/>
       <c r="U147" s="4"/>
       <c r="V147" s="4"/>
-      <c r="W147" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="X147" s="4"/>
+      <c r="W147" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="X147" s="1"/>
       <c r="Y147" s="4"/>
       <c r="Z147" s="4"/>
-      <c r="AA147" s="4" t="s">
-        <v>269</v>
-      </c>
+      <c r="AA147" s="4"/>
       <c r="AB147" s="4"/>
       <c r="AC147" s="2"/>
     </row>
     <row r="148" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A148" s="6"/>
       <c r="B148" s="4"/>
-      <c r="C148" s="4"/>
-      <c r="D148" s="4"/>
+      <c r="C148" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D148" s="18"/>
       <c r="E148" s="4"/>
       <c r="F148" s="4"/>
       <c r="G148" s="4"/>
@@ -6777,22 +6853,22 @@
       <c r="U148" s="4"/>
       <c r="V148" s="4"/>
       <c r="W148" s="21" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="X148" s="21"/>
       <c r="Y148" s="4"/>
       <c r="Z148" s="4"/>
-      <c r="AA148" s="4" t="s">
-        <v>267</v>
-      </c>
+      <c r="AA148" s="4"/>
       <c r="AB148" s="4"/>
       <c r="AC148" s="2"/>
     </row>
     <row r="149" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A149" s="6"/>
       <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
+      <c r="C149" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="D149" s="18"/>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
       <c r="G149" s="4"/>
@@ -6812,7 +6888,7 @@
       <c r="U149" s="4"/>
       <c r="V149" s="4"/>
       <c r="W149" s="21" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="X149" s="21"/>
       <c r="Y149" s="4"/>
@@ -6824,8 +6900,10 @@
     <row r="150" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A150" s="6"/>
       <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
-      <c r="D150" s="4"/>
+      <c r="C150" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="D150" s="18"/>
       <c r="E150" s="4"/>
       <c r="F150" s="4"/>
       <c r="G150" s="4"/>
@@ -6849,7 +6927,7 @@
       <c r="Y150" s="4"/>
       <c r="Z150" s="4"/>
       <c r="AA150" s="21" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="AB150" s="21"/>
       <c r="AC150" s="2"/>
@@ -6857,36 +6935,50 @@
     <row r="151" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A151" s="6"/>
       <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
+      <c r="C151" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
       <c r="F151" s="4"/>
-      <c r="G151" s="4"/>
+      <c r="G151" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
       <c r="J151" s="4"/>
-      <c r="K151" s="4"/>
+      <c r="K151" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="L151" s="4"/>
       <c r="M151" s="4"/>
       <c r="N151" s="4"/>
-      <c r="O151" s="4"/>
+      <c r="O151" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="P151" s="4"/>
       <c r="Q151" s="4"/>
       <c r="R151" s="4"/>
-      <c r="S151" s="4"/>
+      <c r="S151" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="T151" s="4"/>
       <c r="U151" s="4"/>
       <c r="V151" s="4"/>
-      <c r="W151" s="4"/>
+      <c r="W151" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="X151" s="4"/>
       <c r="Y151" s="4"/>
       <c r="Z151" s="4"/>
-      <c r="AA151" s="4"/>
+      <c r="AA151" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="AB151" s="4"/>
       <c r="AC151" s="2"/>
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A152" s="45" t="s">
+      <c r="A152" s="44" t="s">
         <v>217</v>
       </c>
       <c r="B152" s="6"/>
@@ -6935,42 +7027,42 @@
     <row r="153" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A153" s="6"/>
       <c r="B153" s="4"/>
-      <c r="C153" t="s">
-        <v>270</v>
+      <c r="C153" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="E153" s="4"/>
       <c r="F153" s="4"/>
       <c r="G153" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
       <c r="J153" s="4"/>
       <c r="K153" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L153" s="4"/>
       <c r="M153" s="4"/>
       <c r="N153" s="4"/>
       <c r="O153" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="P153" s="4"/>
       <c r="Q153" s="4"/>
       <c r="R153" s="4"/>
       <c r="S153" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="T153" s="4"/>
       <c r="U153" s="4"/>
       <c r="V153" s="4"/>
       <c r="W153" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="Y153" s="4"/>
       <c r="Z153" s="4"/>
       <c r="AA153" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AB153" s="4"/>
       <c r="AC153" s="2"/>
@@ -6979,7 +7071,7 @@
       <c r="A154" s="6"/>
       <c r="B154" s="4"/>
       <c r="C154" t="s">
-        <v>271</v>
+        <v>347</v>
       </c>
       <c r="E154" s="4"/>
       <c r="F154" s="4"/>
@@ -6987,7 +7079,9 @@
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
-      <c r="K154" s="4"/>
+      <c r="K154" s="4" t="s">
+        <v>357</v>
+      </c>
       <c r="L154" s="4"/>
       <c r="M154" s="4"/>
       <c r="N154" s="4"/>
@@ -6995,19 +7089,19 @@
       <c r="P154" s="4"/>
       <c r="Q154" s="4"/>
       <c r="R154" s="4"/>
-      <c r="S154" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="T154" s="4"/>
+      <c r="S154" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="T154" s="1"/>
       <c r="U154" s="4"/>
       <c r="V154" s="4"/>
       <c r="W154" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="Y154" s="4"/>
       <c r="Z154" s="4"/>
       <c r="AA154" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AB154" s="4"/>
       <c r="AC154" s="2"/>
@@ -7015,16 +7109,19 @@
     <row r="155" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A155" s="6"/>
       <c r="B155" s="4"/>
-      <c r="C155" t="s">
-        <v>272</v>
-      </c>
+      <c r="C155" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D155" s="4"/>
       <c r="E155" s="4"/>
       <c r="F155" s="4"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
       <c r="J155" s="4"/>
-      <c r="K155" s="4"/>
+      <c r="K155" s="4" t="s">
+        <v>360</v>
+      </c>
       <c r="L155" s="4"/>
       <c r="M155" s="4"/>
       <c r="N155" s="4"/>
@@ -7032,19 +7129,20 @@
       <c r="P155" s="4"/>
       <c r="Q155" s="4"/>
       <c r="R155" s="4"/>
-      <c r="S155" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="T155" s="4"/>
+      <c r="S155" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="T155" s="1"/>
       <c r="U155" s="4"/>
       <c r="V155" s="4"/>
-      <c r="W155" t="s">
-        <v>291</v>
-      </c>
+      <c r="W155" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="X155" s="46"/>
       <c r="Y155" s="4"/>
       <c r="Z155" s="4"/>
       <c r="AA155" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AB155" s="4"/>
       <c r="AC155" s="2"/>
@@ -7052,9 +7150,10 @@
     <row r="156" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A156" s="10"/>
       <c r="B156" s="2"/>
-      <c r="C156" t="s">
-        <v>273</v>
-      </c>
+      <c r="C156" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D156" s="4"/>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
@@ -7069,686 +7168,801 @@
       <c r="P156" s="2"/>
       <c r="Q156" s="2"/>
       <c r="R156" s="2"/>
-      <c r="S156" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="T156" s="2"/>
+      <c r="S156" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="T156" s="1"/>
       <c r="U156" s="2"/>
       <c r="V156" s="2"/>
-      <c r="W156" t="s">
-        <v>292</v>
-      </c>
       <c r="Y156" s="2"/>
       <c r="Z156" s="4"/>
       <c r="AA156" s="4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="AB156" s="4"/>
       <c r="AC156" s="2"/>
     </row>
     <row r="157" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A157" s="10"/>
-      <c r="C157" t="s">
-        <v>274</v>
-      </c>
-      <c r="W157" t="s">
-        <v>293</v>
+      <c r="C157" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D157" s="4"/>
+      <c r="S157" s="4" t="s">
+        <v>353</v>
       </c>
       <c r="Z157" s="2"/>
       <c r="AA157" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB157" s="2"/>
       <c r="AC157" s="2"/>
     </row>
     <row r="158" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A158" s="10"/>
-      <c r="C158" t="s">
-        <v>275</v>
+      <c r="C158" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D158" s="4"/>
+      <c r="S158" s="4" t="s">
+        <v>354</v>
       </c>
       <c r="W158" s="4"/>
       <c r="Z158" s="2"/>
       <c r="AA158" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AB158" s="2"/>
       <c r="AC158" s="2"/>
     </row>
     <row r="159" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A159" s="10"/>
+      <c r="C159" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D159" s="4"/>
+      <c r="S159" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="W159" s="4"/>
       <c r="Z159" s="2"/>
-      <c r="AA159" s="2"/>
+      <c r="AA159" s="4" t="s">
+        <v>350</v>
+      </c>
       <c r="AB159" s="2"/>
       <c r="AC159" s="2"/>
     </row>
     <row r="160" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A160" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="B160" s="6"/>
-      <c r="C160" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D160" s="6"/>
-      <c r="E160" s="6"/>
-      <c r="F160" s="6"/>
-      <c r="G160" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H160" s="6"/>
-      <c r="I160" s="6"/>
-      <c r="J160" s="6"/>
-      <c r="K160" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L160" s="6"/>
-      <c r="M160" s="6"/>
-      <c r="N160" s="6"/>
-      <c r="O160" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P160" s="6"/>
-      <c r="Q160" s="6"/>
-      <c r="R160" s="6"/>
-      <c r="S160" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="T160" s="6"/>
-      <c r="U160" s="6"/>
-      <c r="V160" s="6"/>
-      <c r="W160" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X160" s="6"/>
-      <c r="Y160" s="6"/>
-      <c r="Z160" s="6"/>
-      <c r="AA160" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB160" s="6"/>
+      <c r="A160" s="10"/>
+      <c r="C160" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D160" s="18"/>
+      <c r="W160" s="4"/>
+      <c r="Z160" s="2"/>
+      <c r="AA160" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="AB160" s="2"/>
       <c r="AC160" s="2"/>
     </row>
     <row r="161" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A161" s="10"/>
       <c r="C161" t="s">
-        <v>279</v>
-      </c>
-      <c r="J161" s="4"/>
-      <c r="K161" s="4"/>
-      <c r="S161" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="T161" s="4"/>
-      <c r="W161" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z161" s="4"/>
+        <v>290</v>
+      </c>
+      <c r="W161" s="4"/>
+      <c r="Z161" s="2"/>
       <c r="AA161" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="AB161" s="4"/>
+        <v>352</v>
+      </c>
+      <c r="AB161" s="2"/>
       <c r="AC161" s="2"/>
     </row>
     <row r="162" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A162" s="45"/>
+      <c r="A162" s="10"/>
       <c r="C162" t="s">
-        <v>280</v>
-      </c>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
-      <c r="S162" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="T162" s="4"/>
-      <c r="W162" t="s">
-        <v>250</v>
-      </c>
-      <c r="Z162" s="4"/>
-      <c r="AA162" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="AB162" s="4"/>
+        <v>291</v>
+      </c>
+      <c r="Z162" s="2"/>
+      <c r="AA162" s="2"/>
+      <c r="AB162" s="2"/>
       <c r="AC162" s="2"/>
     </row>
     <row r="163" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A163" s="10"/>
-      <c r="C163" t="s">
-        <v>281</v>
-      </c>
-      <c r="J163" s="4"/>
-      <c r="K163" s="4"/>
-      <c r="S163" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="T163" s="4"/>
-      <c r="W163" t="s">
-        <v>297</v>
-      </c>
-      <c r="Z163" s="4"/>
-      <c r="AA163" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="AB163" s="4"/>
+      <c r="A163" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="B163" s="6"/>
+      <c r="C163" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D163" s="6"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H163" s="6"/>
+      <c r="I163" s="6"/>
+      <c r="J163" s="6"/>
+      <c r="K163" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L163" s="6"/>
+      <c r="M163" s="6"/>
+      <c r="N163" s="6"/>
+      <c r="O163" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P163" s="6"/>
+      <c r="Q163" s="6"/>
+      <c r="R163" s="6"/>
+      <c r="S163" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T163" s="6"/>
+      <c r="U163" s="6"/>
+      <c r="V163" s="6"/>
+      <c r="W163" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X163" s="6"/>
+      <c r="Y163" s="6"/>
+      <c r="Z163" s="6"/>
+      <c r="AA163" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB163" s="6"/>
       <c r="AC163" s="2"/>
     </row>
     <row r="164" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A164" s="10"/>
       <c r="C164" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
+      <c r="K164" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="L164" s="4"/>
+      <c r="S164" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="T164" s="4"/>
       <c r="W164" t="s">
-        <v>298</v>
+        <v>247</v>
       </c>
       <c r="Z164" s="4"/>
       <c r="AA164" s="4" t="s">
-        <v>262</v>
+        <v>320</v>
       </c>
       <c r="AB164" s="4"/>
       <c r="AC164" s="2"/>
     </row>
     <row r="165" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A165" s="45"/>
+      <c r="A165" s="44"/>
       <c r="C165" t="s">
-        <v>282</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="J165" s="4"/>
+      <c r="K165" s="4"/>
+      <c r="S165" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="T165" s="4"/>
       <c r="W165" t="s">
-        <v>299</v>
-      </c>
-      <c r="Z165" s="2"/>
+        <v>248</v>
+      </c>
+      <c r="Z165" s="4"/>
       <c r="AA165" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="AB165" s="2"/>
+        <v>298</v>
+      </c>
+      <c r="AB165" s="4"/>
       <c r="AC165" s="2"/>
     </row>
     <row r="166" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A166" s="10"/>
       <c r="C166" t="s">
-        <v>283</v>
-      </c>
-      <c r="W166" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="X166" s="20"/>
-      <c r="Z166" s="2"/>
+        <v>279</v>
+      </c>
+      <c r="J166" s="4"/>
+      <c r="K166" s="4"/>
+      <c r="S166" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="T166" s="4"/>
+      <c r="W166" t="s">
+        <v>295</v>
+      </c>
+      <c r="Z166" s="4"/>
       <c r="AA166" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="AB166" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="AB166" s="4"/>
       <c r="AC166" s="2"/>
     </row>
     <row r="167" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A167" s="10"/>
-      <c r="W167" s="20" t="s">
-        <v>338</v>
-      </c>
-      <c r="X167" s="20"/>
-      <c r="Z167" s="2"/>
-      <c r="AA167" s="21" t="s">
-        <v>340</v>
-      </c>
-      <c r="AB167" s="21"/>
+      <c r="C167" t="s">
+        <v>282</v>
+      </c>
+      <c r="J167" s="4"/>
+      <c r="K167" s="4"/>
+      <c r="W167" t="s">
+        <v>296</v>
+      </c>
+      <c r="Z167" s="4"/>
+      <c r="AA167" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB167" s="4"/>
       <c r="AC167" s="2"/>
     </row>
     <row r="168" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A168" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="B168" s="6"/>
-      <c r="C168" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D168" s="6"/>
-      <c r="E168" s="6"/>
-      <c r="F168" s="6"/>
-      <c r="G168" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H168" s="6"/>
-      <c r="I168" s="6"/>
-      <c r="J168" s="6"/>
-      <c r="K168" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L168" s="6"/>
-      <c r="M168" s="6"/>
-      <c r="N168" s="6"/>
-      <c r="O168" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P168" s="6"/>
-      <c r="Q168" s="6"/>
-      <c r="R168" s="6"/>
-      <c r="S168" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="T168" s="6"/>
-      <c r="U168" s="6"/>
-      <c r="V168" s="6"/>
-      <c r="W168" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X168" s="6"/>
-      <c r="Y168" s="6"/>
-      <c r="Z168" s="6"/>
-      <c r="AA168" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB168" s="6"/>
+      <c r="A168" s="44"/>
+      <c r="C168" t="s">
+        <v>280</v>
+      </c>
+      <c r="W168" t="s">
+        <v>297</v>
+      </c>
+      <c r="Z168" s="2"/>
+      <c r="AA168" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="AB168" s="2"/>
       <c r="AC168" s="2"/>
     </row>
     <row r="169" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A169" s="10"/>
       <c r="C169" t="s">
-        <v>276</v>
-      </c>
-      <c r="G169" s="4"/>
-      <c r="H169" s="4"/>
-      <c r="S169" t="s">
-        <v>258</v>
-      </c>
-      <c r="W169" t="s">
-        <v>312</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="W169" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="X169" s="20"/>
       <c r="Z169" s="2"/>
       <c r="AA169" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="AB169" s="4"/>
+        <v>261</v>
+      </c>
+      <c r="AB169" s="2"/>
       <c r="AC169" s="2"/>
     </row>
     <row r="170" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A170" s="10"/>
-      <c r="C170" t="s">
-        <v>277</v>
-      </c>
-      <c r="G170" s="4"/>
-      <c r="H170" s="4"/>
-      <c r="S170" t="s">
-        <v>259</v>
-      </c>
-      <c r="W170" t="s">
-        <v>313</v>
-      </c>
+      <c r="W170" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="X170" s="20"/>
       <c r="Z170" s="2"/>
-      <c r="AA170" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="AB170" s="4"/>
+      <c r="AA170" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="AB170" s="21"/>
       <c r="AC170" s="2"/>
     </row>
     <row r="171" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A171" s="10"/>
       <c r="C171" t="s">
-        <v>278</v>
-      </c>
-      <c r="G171" s="4"/>
-      <c r="H171" s="4"/>
-      <c r="S171" t="s">
-        <v>260</v>
-      </c>
-      <c r="Z171" s="2"/>
-      <c r="AA171" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="AB171" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="W171" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="X171" s="46"/>
+      <c r="Y171" s="46"/>
+      <c r="Z171" s="4"/>
+      <c r="AA171" s="4"/>
+      <c r="AB171" s="4"/>
       <c r="AC171" s="2"/>
     </row>
     <row r="172" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A172" s="10"/>
-      <c r="C172" s="4"/>
-      <c r="D172" s="4"/>
-      <c r="G172" s="4"/>
-      <c r="H172" s="2"/>
-      <c r="Z172" s="2"/>
-      <c r="AA172" s="2"/>
-      <c r="AB172" s="2"/>
+      <c r="A172" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="B172" s="6"/>
+      <c r="C172" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D172" s="6"/>
+      <c r="E172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H172" s="6"/>
+      <c r="I172" s="6"/>
+      <c r="J172" s="6"/>
+      <c r="K172" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L172" s="6"/>
+      <c r="M172" s="6"/>
+      <c r="N172" s="6"/>
+      <c r="O172" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P172" s="6"/>
+      <c r="Q172" s="6"/>
+      <c r="R172" s="6"/>
+      <c r="S172" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T172" s="6"/>
+      <c r="U172" s="6"/>
+      <c r="V172" s="6"/>
+      <c r="W172" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X172" s="6"/>
+      <c r="Y172" s="6"/>
+      <c r="Z172" s="6"/>
+      <c r="AA172" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB172" s="6"/>
       <c r="AC172" s="2"/>
     </row>
     <row r="173" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A173" s="10"/>
+      <c r="C173" t="s">
+        <v>274</v>
+      </c>
       <c r="G173" s="4"/>
+      <c r="H173" s="4"/>
+      <c r="K173" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="L173" s="4"/>
+      <c r="S173" t="s">
+        <v>256</v>
+      </c>
+      <c r="W173" t="s">
+        <v>310</v>
+      </c>
       <c r="Z173" s="2"/>
-      <c r="AA173" s="2"/>
-      <c r="AB173" s="2"/>
+      <c r="AA173" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="AB173" s="4"/>
       <c r="AC173" s="2"/>
     </row>
     <row r="174" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A174" s="10"/>
+      <c r="C174" t="s">
+        <v>275</v>
+      </c>
       <c r="G174" s="4"/>
+      <c r="H174" s="4"/>
+      <c r="S174" t="s">
+        <v>257</v>
+      </c>
+      <c r="W174" t="s">
+        <v>311</v>
+      </c>
       <c r="Z174" s="2"/>
-      <c r="AA174" s="2"/>
-      <c r="AB174" s="2"/>
+      <c r="AA174" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="AB174" s="4"/>
       <c r="AC174" s="2"/>
     </row>
     <row r="175" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A175" s="10"/>
+      <c r="C175" t="s">
+        <v>276</v>
+      </c>
+      <c r="G175" s="4"/>
+      <c r="H175" s="4"/>
+      <c r="S175" t="s">
+        <v>258</v>
+      </c>
+      <c r="W175" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="X175" s="46"/>
       <c r="Z175" s="2"/>
-      <c r="AA175" s="2"/>
+      <c r="AA175" s="4" t="s">
+        <v>303</v>
+      </c>
       <c r="AB175" s="2"/>
       <c r="AC175" s="2"/>
     </row>
     <row r="176" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A176" s="45" t="s">
-        <v>220</v>
-      </c>
-      <c r="B176" s="6"/>
-      <c r="C176" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D176" s="6"/>
-      <c r="E176" s="6"/>
-      <c r="F176" s="6"/>
-      <c r="G176" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H176" s="6"/>
-      <c r="I176" s="6"/>
-      <c r="J176" s="6"/>
-      <c r="K176" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L176" s="6"/>
-      <c r="M176" s="6"/>
-      <c r="N176" s="6"/>
-      <c r="O176" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P176" s="6"/>
-      <c r="Q176" s="6"/>
-      <c r="R176" s="6"/>
-      <c r="S176" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="T176" s="6"/>
-      <c r="U176" s="6"/>
-      <c r="V176" s="6"/>
-      <c r="W176" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X176" s="6"/>
-      <c r="Y176" s="6"/>
-      <c r="Z176" s="6"/>
-      <c r="AA176" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB176" s="6"/>
+      <c r="A176" s="10"/>
+      <c r="C176" s="4"/>
+      <c r="D176" s="4"/>
+      <c r="G176" s="4"/>
+      <c r="H176" s="2"/>
+      <c r="Z176" s="2"/>
+      <c r="AA176" s="2"/>
+      <c r="AB176" s="2"/>
       <c r="AC176" s="2"/>
     </row>
     <row r="177" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A177" s="10"/>
-      <c r="C177" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D177" s="4"/>
       <c r="G177" s="4"/>
-      <c r="H177" s="4"/>
-      <c r="S177" t="s">
-        <v>300</v>
-      </c>
-      <c r="W177" t="s">
-        <v>285</v>
-      </c>
       <c r="Z177" s="2"/>
-      <c r="AA177" t="s">
-        <v>264</v>
-      </c>
+      <c r="AA177" s="2"/>
+      <c r="AB177" s="2"/>
       <c r="AC177" s="2"/>
     </row>
     <row r="178" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A178" s="10"/>
-      <c r="C178" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D178" s="4"/>
       <c r="G178" s="4"/>
-      <c r="H178" s="4"/>
-      <c r="S178" t="s">
-        <v>301</v>
-      </c>
-      <c r="W178" t="s">
-        <v>286</v>
-      </c>
       <c r="Z178" s="2"/>
-      <c r="AA178" t="s">
-        <v>265</v>
-      </c>
+      <c r="AA178" s="2"/>
+      <c r="AB178" s="2"/>
       <c r="AC178" s="2"/>
     </row>
     <row r="179" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A179" s="10"/>
-      <c r="C179" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D179" s="4"/>
-      <c r="G179" s="4"/>
-      <c r="H179" s="4"/>
-      <c r="S179" t="s">
-        <v>302</v>
-      </c>
-      <c r="W179" t="s">
-        <v>287</v>
-      </c>
-      <c r="AA179" t="s">
-        <v>266</v>
-      </c>
+      <c r="Z179" s="2"/>
+      <c r="AA179" s="2"/>
+      <c r="AB179" s="2"/>
+      <c r="AC179" s="2"/>
     </row>
     <row r="180" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A180" s="10"/>
-      <c r="C180" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D180" s="4"/>
-      <c r="G180" s="4"/>
-      <c r="H180" s="4"/>
-      <c r="W180" t="s">
-        <v>288</v>
-      </c>
+      <c r="A180" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="B180" s="6"/>
+      <c r="C180" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D180" s="6"/>
+      <c r="E180" s="6"/>
+      <c r="F180" s="6"/>
+      <c r="G180" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H180" s="6"/>
+      <c r="I180" s="6"/>
+      <c r="J180" s="6"/>
+      <c r="K180" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L180" s="6"/>
+      <c r="M180" s="6"/>
+      <c r="N180" s="6"/>
+      <c r="O180" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P180" s="6"/>
+      <c r="Q180" s="6"/>
+      <c r="R180" s="6"/>
+      <c r="S180" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T180" s="6"/>
+      <c r="U180" s="6"/>
+      <c r="V180" s="6"/>
+      <c r="W180" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X180" s="6"/>
+      <c r="Y180" s="6"/>
+      <c r="Z180" s="6"/>
+      <c r="AA180" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB180" s="6"/>
+      <c r="AC180" s="2"/>
     </row>
     <row r="181" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A181" s="10"/>
+      <c r="C181" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D181" s="4"/>
+      <c r="G181" s="4"/>
+      <c r="H181" s="4"/>
+      <c r="K181" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="L181" s="4"/>
+      <c r="S181" t="s">
+        <v>298</v>
+      </c>
       <c r="W181" t="s">
-        <v>289</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="Z181" s="2"/>
+      <c r="AA181" t="s">
+        <v>262</v>
+      </c>
+      <c r="AC181" s="2"/>
     </row>
     <row r="182" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A182" s="10"/>
+      <c r="C182" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D182" s="4"/>
+      <c r="G182" s="4"/>
+      <c r="H182" s="4"/>
+      <c r="S182" t="s">
+        <v>299</v>
+      </c>
       <c r="W182" t="s">
-        <v>290</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="Z182" s="2"/>
+      <c r="AA182" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC182" s="2"/>
     </row>
     <row r="183" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A183" s="10"/>
-      <c r="W183" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="X183" s="20"/>
-      <c r="AA183" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="AB183" s="20"/>
+      <c r="C183" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D183" s="4"/>
+      <c r="G183" s="4"/>
+      <c r="H183" s="4"/>
+      <c r="S183" t="s">
+        <v>300</v>
+      </c>
+      <c r="W183" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA183" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="184" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A184" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="B184" s="6"/>
-      <c r="C184" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D184" s="6"/>
-      <c r="E184" s="6"/>
-      <c r="F184" s="6"/>
-      <c r="G184" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H184" s="6"/>
-      <c r="I184" s="6"/>
-      <c r="J184" s="6"/>
-      <c r="K184" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L184" s="6"/>
-      <c r="M184" s="6"/>
-      <c r="N184" s="6"/>
-      <c r="O184" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P184" s="6"/>
-      <c r="Q184" s="6"/>
-      <c r="R184" s="6"/>
-      <c r="S184" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="T184" s="6"/>
-      <c r="U184" s="6"/>
-      <c r="V184" s="6"/>
-      <c r="W184" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X184" s="6"/>
-      <c r="Y184" s="6"/>
-      <c r="Z184" s="6"/>
-      <c r="AA184" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB184" s="15"/>
+      <c r="A184" s="10"/>
+      <c r="C184" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D184" s="4"/>
+      <c r="G184" s="4"/>
+      <c r="H184" s="4"/>
+      <c r="S184" t="s">
+        <v>314</v>
+      </c>
+      <c r="W184" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="185" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A185" s="10"/>
       <c r="S185" t="s">
-        <v>317</v>
+        <v>315</v>
+      </c>
+      <c r="W185" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="186" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A186" s="10"/>
-      <c r="S186" t="s">
-        <v>318</v>
+      <c r="W186" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="187" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A187" s="10"/>
+      <c r="W187" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="X187" s="20"/>
+      <c r="AA187" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="AB187" s="20"/>
     </row>
     <row r="188" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A188" s="10"/>
-    </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A188" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="B188" s="6"/>
+      <c r="C188" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D188" s="6"/>
+      <c r="E188" s="6"/>
+      <c r="F188" s="6"/>
+      <c r="G188" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H188" s="6"/>
+      <c r="I188" s="6"/>
+      <c r="J188" s="6"/>
+      <c r="K188" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L188" s="6"/>
+      <c r="M188" s="6"/>
+      <c r="N188" s="6"/>
+      <c r="O188" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P188" s="6"/>
+      <c r="Q188" s="6"/>
+      <c r="R188" s="6"/>
+      <c r="S188" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T188" s="6"/>
+      <c r="U188" s="6"/>
+      <c r="V188" s="6"/>
+      <c r="W188" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X188" s="6"/>
+      <c r="Y188" s="6"/>
+      <c r="Z188" s="6"/>
+      <c r="AA188" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB188" s="15"/>
+    </row>
+    <row r="189" spans="1:29" ht="51" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A189" s="10"/>
+      <c r="D189" s="45" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="190" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A190" s="10"/>
+      <c r="A190" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B190" s="6"/>
+      <c r="C190" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D190" s="6"/>
+      <c r="E190" s="6"/>
+      <c r="F190" s="6"/>
+      <c r="G190" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H190" s="6"/>
+      <c r="I190" s="6"/>
+      <c r="J190" s="6"/>
+      <c r="K190" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L190" s="6"/>
+      <c r="M190" s="6"/>
+      <c r="N190" s="6"/>
+      <c r="O190" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P190" s="6"/>
+      <c r="Q190" s="6"/>
+      <c r="R190" s="6"/>
+      <c r="S190" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T190" s="6"/>
+      <c r="U190" s="6"/>
+      <c r="V190" s="6"/>
+      <c r="W190" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X190" s="6"/>
+      <c r="Y190" s="6"/>
+      <c r="Z190" s="6"/>
+      <c r="AA190" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB190" s="15"/>
     </row>
     <row r="191" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A191" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="B191" s="6"/>
-      <c r="C191" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D191" s="6"/>
-      <c r="E191" s="6"/>
-      <c r="F191" s="6"/>
-      <c r="G191" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H191" s="6"/>
-      <c r="I191" s="6"/>
-      <c r="J191" s="6"/>
-      <c r="K191" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L191" s="6"/>
-      <c r="M191" s="6"/>
-      <c r="N191" s="6"/>
-      <c r="O191" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P191" s="6"/>
-      <c r="Q191" s="6"/>
-      <c r="R191" s="6"/>
-      <c r="S191" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="T191" s="6"/>
-      <c r="U191" s="6"/>
-      <c r="V191" s="6"/>
-      <c r="W191" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X191" s="6"/>
-      <c r="Y191" s="6"/>
-      <c r="Z191" s="6"/>
-      <c r="AA191" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB191" s="15"/>
-    </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A191" s="10"/>
+    </row>
+    <row r="192" spans="1:29" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A192" s="10"/>
+      <c r="D192" s="45" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="193" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A193" s="10"/>
     </row>
     <row r="194" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A194" s="10"/>
+      <c r="A194" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D194" s="6"/>
+      <c r="E194" s="6"/>
+      <c r="F194" s="6"/>
+      <c r="G194" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H194" s="6"/>
+      <c r="I194" s="6"/>
+      <c r="J194" s="6"/>
+      <c r="K194" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L194" s="6"/>
+      <c r="M194" s="6"/>
+      <c r="N194" s="6"/>
+      <c r="O194" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P194" s="6"/>
+      <c r="Q194" s="6"/>
+      <c r="R194" s="6"/>
+      <c r="S194" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T194" s="6"/>
+      <c r="U194" s="6"/>
+      <c r="V194" s="6"/>
+      <c r="W194" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X194" s="6"/>
+      <c r="Y194" s="6"/>
+      <c r="Z194" s="6"/>
+      <c r="AA194" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB194" s="15"/>
     </row>
     <row r="195" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A195" s="10"/>
+      <c r="C195" t="s">
+        <v>358</v>
+      </c>
+      <c r="G195" t="s">
+        <v>358</v>
+      </c>
+      <c r="K195" t="s">
+        <v>358</v>
+      </c>
+      <c r="O195" t="s">
+        <v>358</v>
+      </c>
+      <c r="S195" t="s">
+        <v>358</v>
+      </c>
+      <c r="W195" t="s">
+        <v>358</v>
+      </c>
+      <c r="AA195" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="196" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A196" s="10"/>
+      <c r="C196" t="s">
+        <v>359</v>
+      </c>
+      <c r="G196" t="s">
+        <v>359</v>
+      </c>
+      <c r="K196" t="s">
+        <v>359</v>
+      </c>
+      <c r="O196" t="s">
+        <v>359</v>
+      </c>
+      <c r="S196" t="s">
+        <v>359</v>
+      </c>
+      <c r="W196" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA196" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="197" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A197" s="10"/>
     </row>
     <row r="198" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A198" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="B198" s="6"/>
-      <c r="C198" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D198" s="6"/>
-      <c r="E198" s="6"/>
-      <c r="F198" s="6"/>
-      <c r="G198" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H198" s="6"/>
-      <c r="I198" s="6"/>
-      <c r="J198" s="6"/>
-      <c r="K198" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L198" s="6"/>
-      <c r="M198" s="6"/>
-      <c r="N198" s="6"/>
-      <c r="O198" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P198" s="6"/>
-      <c r="Q198" s="6"/>
-      <c r="R198" s="6"/>
-      <c r="S198" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="T198" s="6"/>
-      <c r="U198" s="6"/>
-      <c r="V198" s="6"/>
-      <c r="W198" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X198" s="6"/>
-      <c r="Y198" s="6"/>
-      <c r="Z198" s="6"/>
-      <c r="AA198" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB198" s="15"/>
+      <c r="A198" s="10"/>
     </row>
     <row r="199" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A199" s="10"/>
@@ -7757,20 +7971,139 @@
       <c r="A200" s="10"/>
     </row>
     <row r="201" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A201" s="10"/>
+      <c r="A201" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B201" s="6"/>
+      <c r="C201" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D201" s="6"/>
+      <c r="E201" s="6"/>
+      <c r="F201" s="6"/>
+      <c r="G201" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H201" s="6"/>
+      <c r="I201" s="6"/>
+      <c r="J201" s="6"/>
+      <c r="K201" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L201" s="6"/>
+      <c r="M201" s="6"/>
+      <c r="N201" s="6"/>
+      <c r="O201" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P201" s="6"/>
+      <c r="Q201" s="6"/>
+      <c r="R201" s="6"/>
+      <c r="S201" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T201" s="6"/>
+      <c r="U201" s="6"/>
+      <c r="V201" s="6"/>
+      <c r="W201" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X201" s="6"/>
+      <c r="Y201" s="6"/>
+      <c r="Z201" s="6"/>
+      <c r="AA201" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB201" s="15"/>
     </row>
     <row r="202" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A202" s="10"/>
-    </row>
-    <row r="203" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B202" s="4"/>
+      <c r="C202" t="s">
+        <v>359</v>
+      </c>
+      <c r="G202" t="s">
+        <v>359</v>
+      </c>
+      <c r="K202" t="s">
+        <v>359</v>
+      </c>
+      <c r="O202" t="s">
+        <v>359</v>
+      </c>
+      <c r="S202" t="s">
+        <v>359</v>
+      </c>
+      <c r="W202" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA202" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="203" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="10"/>
-    </row>
-    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B203" s="4"/>
+      <c r="C203" s="4"/>
+      <c r="D203" s="4"/>
+      <c r="E203" s="4"/>
+      <c r="F203" s="4"/>
+      <c r="G203" s="4"/>
+      <c r="H203" s="4"/>
+      <c r="I203" s="4"/>
+      <c r="J203" s="4"/>
+      <c r="K203" s="4"/>
+      <c r="L203" s="4"/>
+      <c r="M203" s="4"/>
+      <c r="N203" s="4"/>
+      <c r="O203" s="4"/>
+      <c r="P203" s="4"/>
+      <c r="Q203" s="4"/>
+      <c r="R203" s="4"/>
+      <c r="S203" s="4"/>
+      <c r="T203" s="4"/>
+      <c r="U203" s="4"/>
+      <c r="V203" s="4"/>
+      <c r="W203" s="4"/>
+      <c r="X203" s="4"/>
+      <c r="Y203" s="4"/>
+      <c r="Z203" s="4"/>
+      <c r="AA203" s="4"/>
+      <c r="AB203" s="4"/>
+    </row>
+    <row r="204" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A204" s="10"/>
+      <c r="B204" s="41"/>
+      <c r="C204" s="47"/>
+      <c r="D204" s="48"/>
+      <c r="E204" s="48"/>
+      <c r="F204" s="48"/>
+      <c r="G204" s="47"/>
+      <c r="H204" s="48"/>
+      <c r="I204" s="48"/>
+      <c r="J204" s="48"/>
+      <c r="K204" s="47"/>
+      <c r="L204" s="48"/>
+      <c r="M204" s="48"/>
+      <c r="N204" s="48"/>
+      <c r="O204" s="48"/>
+      <c r="P204" s="47"/>
+      <c r="Q204" s="48"/>
+      <c r="R204" s="48"/>
+      <c r="S204" s="48"/>
+      <c r="T204" s="48"/>
+      <c r="U204" s="47"/>
+      <c r="V204" s="48"/>
+      <c r="W204" s="48"/>
+      <c r="X204" s="48"/>
+      <c r="Y204" s="47"/>
+      <c r="Z204" s="48"/>
+      <c r="AA204" s="48"/>
+      <c r="AB204" s="42"/>
     </row>
     <row r="205" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A205" s="10" t="s">
-        <v>224</v>
+        <v>342</v>
       </c>
       <c r="B205" s="6"/>
       <c r="C205" s="6" t="s">
@@ -7814,91 +8147,79 @@
       </c>
       <c r="AB205" s="15"/>
     </row>
-    <row r="206" spans="1:28" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A206" s="10"/>
-      <c r="B206" s="41"/>
-      <c r="C206" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="D206" s="43"/>
-      <c r="E206" s="43"/>
-      <c r="F206" s="43"/>
-      <c r="G206" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="H206" s="43"/>
-      <c r="I206" s="43"/>
-      <c r="J206" s="43"/>
-      <c r="K206" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="L206" s="43"/>
-      <c r="M206" s="43"/>
-      <c r="N206" s="43"/>
-      <c r="O206" s="43"/>
-      <c r="P206" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q206" s="43"/>
-      <c r="R206" s="43"/>
-      <c r="S206" s="43"/>
-      <c r="T206" s="43"/>
-      <c r="U206" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="V206" s="43"/>
-      <c r="W206" s="43"/>
-      <c r="X206" s="43"/>
-      <c r="Y206" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="Z206" s="43"/>
-      <c r="AA206" s="43"/>
-      <c r="AB206" s="43"/>
+    <row r="206" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A206" s="35"/>
+      <c r="C206" t="s">
+        <v>359</v>
+      </c>
+      <c r="G206" t="s">
+        <v>359</v>
+      </c>
+      <c r="K206" t="s">
+        <v>359</v>
+      </c>
+      <c r="O206" t="s">
+        <v>359</v>
+      </c>
+      <c r="S206" t="s">
+        <v>359</v>
+      </c>
+      <c r="W206" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA206" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="207" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A207" s="23"/>
-      <c r="B207" s="24" t="s">
+      <c r="A207" s="35"/>
+    </row>
+    <row r="208" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A208" s="35"/>
+    </row>
+    <row r="209" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A209" s="35"/>
+      <c r="B209" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C207" s="24"/>
-      <c r="D207" s="24"/>
-      <c r="E207" s="24"/>
-      <c r="F207" s="24" t="s">
+      <c r="C209" s="24"/>
+      <c r="D209" s="24"/>
+      <c r="E209" s="24"/>
+      <c r="F209" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G207" s="24"/>
-      <c r="H207" s="24"/>
-      <c r="I207" s="24"/>
-      <c r="J207" s="24" t="s">
+      <c r="G209" s="24"/>
+      <c r="H209" s="24"/>
+      <c r="I209" s="24"/>
+      <c r="J209" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="K207" s="24"/>
-      <c r="L207" s="24"/>
-      <c r="M207" s="24"/>
-      <c r="N207" s="24" t="s">
+      <c r="K209" s="24"/>
+      <c r="L209" s="24"/>
+      <c r="M209" s="24"/>
+      <c r="N209" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="O207" s="24"/>
-      <c r="P207" s="24"/>
-      <c r="Q207" s="24"/>
-      <c r="R207" s="24"/>
-      <c r="S207" s="24" t="s">
+      <c r="O209" s="24"/>
+      <c r="P209" s="24"/>
+      <c r="Q209" s="24"/>
+      <c r="R209" s="24"/>
+      <c r="S209" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="T207" s="24"/>
-      <c r="U207" s="24"/>
-      <c r="V207" s="24"/>
-      <c r="W207" s="24" t="s">
+      <c r="T209" s="24"/>
+      <c r="U209" s="24"/>
+      <c r="V209" s="24"/>
+      <c r="W209" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="X207" s="24"/>
-      <c r="Y207" s="24"/>
-      <c r="Z207" s="24" t="s">
+      <c r="X209" s="24"/>
+      <c r="Y209" s="24"/>
+      <c r="Z209" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA207" s="24"/>
-      <c r="AB207" s="25"/>
+      <c r="AA209" s="24"/>
+      <c r="AB209" s="25"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="V54:X56 W59:W62 W64:W69">

</xml_diff>

<commit_message>
House Texture / Chair / Uren
Objects
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="366">
   <si>
     <t>Planning</t>
   </si>
@@ -1119,6 +1119,9 @@
   </si>
   <si>
     <t>Sarah Fixing</t>
+  </si>
+  <si>
+    <t>MolsPile</t>
   </si>
 </sst>
 </file>
@@ -1732,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AC214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N166" sqref="M166:N169"/>
+    <sheetView tabSelected="1" topLeftCell="C179" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA195" sqref="AA195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7558,9 +7561,10 @@
         <v>358</v>
       </c>
       <c r="L175" s="4"/>
-      <c r="S175" t="s">
+      <c r="S175" s="49" t="s">
         <v>256</v>
       </c>
+      <c r="T175" s="49"/>
       <c r="W175" s="49" t="s">
         <v>309</v>
       </c>
@@ -7580,9 +7584,10 @@
       <c r="D176" s="49"/>
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
-      <c r="S176" t="s">
+      <c r="S176" s="49" t="s">
         <v>257</v>
       </c>
+      <c r="T176" s="49"/>
       <c r="W176" s="49" t="s">
         <v>310</v>
       </c>
@@ -7600,9 +7605,10 @@
       <c r="D177" s="49"/>
       <c r="G177" s="4"/>
       <c r="H177" s="4"/>
-      <c r="S177" t="s">
+      <c r="S177" s="49" t="s">
         <v>258</v>
       </c>
+      <c r="T177" s="49"/>
       <c r="W177" s="46" t="s">
         <v>359</v>
       </c>
@@ -7872,6 +7878,9 @@
       </c>
       <c r="D194" s="45" t="s">
         <v>339</v>
+      </c>
+      <c r="AA194" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="195" spans="1:28" x14ac:dyDescent="0.3">

</xml_diff>